<commit_message>
Exp 1 and 2 improved
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp1_2observed.xlsx
+++ b/Prototypes/Mungbean/Exp1_2observed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A21068-49E0-4A01-9430-5255A5C313C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DB1535-1E8F-46D1-AE22-5BE2BC3CE4F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC5736B7-331A-44E7-9B2A-DE6BDB9CC19C}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:AI574"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="F550" sqref="F549:F550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -838,7 +838,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" hidden="1">
       <c r="B6" t="s">
         <v>51</v>
       </c>
@@ -873,7 +873,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" hidden="1">
       <c r="B7" t="s">
         <v>51</v>
       </c>
@@ -962,7 +962,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" hidden="1">
       <c r="B10" t="s">
         <v>51</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" hidden="1">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" hidden="1">
       <c r="B14" t="s">
         <v>51</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>1.2211347114483</v>
       </c>
       <c r="W35">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="X35">
         <v>0.910796518395528</v>
@@ -2415,7 +2415,7 @@
         <v>6.2934654591232597</v>
       </c>
       <c r="W56">
-        <v>1.47576189158542</v>
+        <v>1.44</v>
       </c>
       <c r="AA56">
         <v>41</v>
@@ -3714,7 +3714,7 @@
         <v>5.6774560370382101</v>
       </c>
       <c r="W95">
-        <v>1.3717302985031801</v>
+        <v>1.56</v>
       </c>
       <c r="Z95">
         <v>0.39576820682952901</v>
@@ -4082,7 +4082,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="2:34" hidden="1">
+    <row r="107" spans="2:34">
       <c r="B107" t="s">
         <v>43</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="125" spans="2:34" hidden="1">
+    <row r="125" spans="2:34">
       <c r="B125" t="s">
         <v>43</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>10.941659688160399</v>
       </c>
       <c r="W125">
-        <v>1.72</v>
+        <v>1.86</v>
       </c>
       <c r="X125">
         <v>8.43</v>
@@ -5040,7 +5040,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="141" spans="2:31">
+    <row r="141" spans="2:31" hidden="1">
       <c r="B141" t="s">
         <v>51</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>63.925992558050403</v>
       </c>
       <c r="W150">
-        <v>0.85430709461809295</v>
+        <v>1.05</v>
       </c>
       <c r="X150">
         <v>3.2913906189906301</v>
@@ -5587,7 +5587,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="160" spans="2:35">
+    <row r="160" spans="2:35" hidden="1">
       <c r="B160" t="s">
         <v>51</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="2:34" hidden="1">
+    <row r="163" spans="2:34">
       <c r="B163" t="s">
         <v>43</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>11.762332017386401</v>
       </c>
       <c r="W163">
-        <v>2.0099999999999998</v>
+        <v>2.08</v>
       </c>
       <c r="X163">
         <v>7.65</v>
@@ -5873,7 +5873,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="169" spans="2:34">
+    <row r="169" spans="2:34" hidden="1">
       <c r="B169" t="s">
         <v>51</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="174" spans="2:34">
+    <row r="174" spans="2:34" hidden="1">
       <c r="B174" t="s">
         <v>51</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="181" spans="2:34">
+    <row r="181" spans="2:34" hidden="1">
       <c r="B181" t="s">
         <v>51</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="2:35" hidden="1">
+    <row r="213" spans="2:35">
       <c r="B213" t="s">
         <v>43</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>15.409020217729299</v>
       </c>
       <c r="W213">
-        <v>1.54</v>
+        <v>1.6</v>
       </c>
       <c r="X213">
         <v>5.04</v>
@@ -7621,7 +7621,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="234" spans="2:35" hidden="1">
+    <row r="234" spans="2:35">
       <c r="B234" t="s">
         <v>43</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="2:32">
+    <row r="279" spans="2:32" hidden="1">
       <c r="B279" t="s">
         <v>51</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>0.20835214446952199</v>
       </c>
       <c r="W283">
-        <v>1.2316725694789299</v>
+        <v>1.43</v>
       </c>
       <c r="X283">
         <v>3.5894638174648099</v>
@@ -9582,7 +9582,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="309" spans="2:29">
+    <row r="309" spans="2:29" hidden="1">
       <c r="B309" t="s">
         <v>51</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="321" spans="2:32">
+    <row r="321" spans="2:32" hidden="1">
       <c r="B321" t="s">
         <v>51</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="333" spans="2:32">
+    <row r="333" spans="2:32" hidden="1">
       <c r="B333" t="s">
         <v>51</v>
       </c>
@@ -11420,7 +11420,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="374" spans="2:35" hidden="1">
+    <row r="374" spans="2:35">
       <c r="B374" t="s">
         <v>43</v>
       </c>
@@ -11434,7 +11434,7 @@
         <v>16.3</v>
       </c>
       <c r="W374">
-        <v>1.96</v>
+        <v>1.97</v>
       </c>
       <c r="X374">
         <v>4.25</v>
@@ -11553,7 +11553,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="379" spans="2:35" hidden="1">
+    <row r="379" spans="2:35">
       <c r="B379" t="s">
         <v>43</v>
       </c>
@@ -11567,7 +11567,7 @@
         <v>15.2560513618056</v>
       </c>
       <c r="W379">
-        <v>1.76</v>
+        <v>1.82</v>
       </c>
       <c r="X379">
         <v>0.38</v>
@@ -12217,7 +12217,7 @@
         <v>0.26027088036117002</v>
       </c>
       <c r="W401">
-        <v>0.96717528708234102</v>
+        <v>1.19</v>
       </c>
       <c r="X401">
         <v>3.1607385726717299</v>
@@ -12441,7 +12441,7 @@
       </c>
       <c r="I409" s="7"/>
       <c r="W409">
-        <v>0.72778880632850396</v>
+        <v>0.83</v>
       </c>
       <c r="Z409">
         <v>7.0658989925840796</v>
@@ -14923,7 +14923,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="496" spans="2:35">
+    <row r="496" spans="2:35" hidden="1">
       <c r="B496" t="s">
         <v>51</v>
       </c>
@@ -14946,7 +14946,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="497" spans="2:35">
+    <row r="497" spans="2:35" hidden="1">
       <c r="B497" t="s">
         <v>51</v>
       </c>
@@ -14975,7 +14975,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="498" spans="2:35">
+    <row r="498" spans="2:35" hidden="1">
       <c r="B498" t="s">
         <v>51</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="499" spans="2:35">
+    <row r="499" spans="2:35" hidden="1">
       <c r="B499" t="s">
         <v>51</v>
       </c>
@@ -15023,7 +15023,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="500" spans="2:35">
+    <row r="500" spans="2:35" hidden="1">
       <c r="B500" t="s">
         <v>51</v>
       </c>
@@ -15055,7 +15055,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="501" spans="2:35">
+    <row r="501" spans="2:35" hidden="1">
       <c r="B501" t="s">
         <v>51</v>
       </c>
@@ -15093,7 +15093,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="502" spans="2:35">
+    <row r="502" spans="2:35" hidden="1">
       <c r="B502" t="s">
         <v>51</v>
       </c>
@@ -15122,7 +15122,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="503" spans="2:35">
+    <row r="503" spans="2:35" hidden="1">
       <c r="B503" t="s">
         <v>51</v>
       </c>
@@ -15145,7 +15145,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="504" spans="2:35">
+    <row r="504" spans="2:35" hidden="1">
       <c r="B504" t="s">
         <v>51</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="505" spans="2:35">
+    <row r="505" spans="2:35" hidden="1">
       <c r="B505" t="s">
         <v>51</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="506" spans="2:35">
+    <row r="506" spans="2:35" hidden="1">
       <c r="B506" t="s">
         <v>51</v>
       </c>
@@ -16123,8 +16123,13 @@
   <autoFilter ref="A1:AI536" xr:uid="{C6959FE3-A6F8-4DED-9137-41C71F649D59}">
     <filterColumn colId="1">
       <filters>
-        <filter val="exp2WaterTermStressCultivarEmerald"/>
+        <filter val="exp1WaterIrrCultivarEmerald"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="22">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AI485">
       <sortCondition ref="G2:G536"/>

</xml_diff>

<commit_message>
Fit model to the point that Neil can look at it.
</commit_message>
<xml_diff>
--- a/Prototypes/Mungbean/Exp1_2observed.xlsx
+++ b/Prototypes/Mungbean/Exp1_2observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Prototypes\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473CC3B3-A87F-4C66-95E0-DADC7B0EE94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD200AC-46CE-4CEA-B771-1C18EF84FC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="6315" windowWidth="20775" windowHeight="11835" xr2:uid="{EC5736B7-331A-44E7-9B2A-DE6BDB9CC19C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{EC5736B7-331A-44E7-9B2A-DE6BDB9CC19C}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -593,10 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C69D9A-1FFA-4799-BC03-A6694D3363DD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI574"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N103" sqref="N103:N104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,7 +713,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" hidden="1">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -747,7 +748,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" hidden="1">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -779,7 +780,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" hidden="1">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -833,9 +834,6 @@
       <c r="AB5">
         <v>49</v>
       </c>
-      <c r="AC5">
-        <v>111</v>
-      </c>
     </row>
     <row r="6" spans="1:35">
       <c r="B6" t="s">
@@ -867,9 +865,6 @@
       </c>
       <c r="AB6">
         <v>49</v>
-      </c>
-      <c r="AC6">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:35">
@@ -911,11 +906,8 @@
       <c r="AB7">
         <v>49</v>
       </c>
-      <c r="AC7">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35">
+    </row>
+    <row r="8" spans="1:35" hidden="1">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -938,7 +930,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" hidden="1">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -989,11 +981,8 @@
       <c r="AB10">
         <v>49</v>
       </c>
-      <c r="AC10">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35">
+    </row>
+    <row r="11" spans="1:35" hidden="1">
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -1064,9 +1053,6 @@
       <c r="AB12">
         <v>49</v>
       </c>
-      <c r="AC12">
-        <v>91</v>
-      </c>
       <c r="AG12">
         <v>7.2</v>
       </c>
@@ -1074,7 +1060,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" hidden="1">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -1122,14 +1108,11 @@
       <c r="AB14">
         <v>49</v>
       </c>
-      <c r="AC14">
-        <v>91</v>
-      </c>
       <c r="AI14">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" hidden="1">
       <c r="B15" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1138,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" hidden="1">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -1178,7 +1161,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="2:35">
+    <row r="17" spans="2:35" hidden="1">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -1204,7 +1187,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="2:35">
+    <row r="18" spans="2:35" hidden="1">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -1246,9 +1229,6 @@
       <c r="AB19">
         <v>49</v>
       </c>
-      <c r="AC19">
-        <v>111</v>
-      </c>
     </row>
     <row r="20" spans="2:35">
       <c r="B20" t="s">
@@ -1275,11 +1255,8 @@
       <c r="AB20">
         <v>49</v>
       </c>
-      <c r="AC20">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="2:35">
+    </row>
+    <row r="21" spans="2:35" hidden="1">
       <c r="B21" t="s">
         <v>15</v>
       </c>
@@ -1339,14 +1316,11 @@
       <c r="AB22">
         <v>49</v>
       </c>
-      <c r="AC22">
-        <v>111</v>
-      </c>
       <c r="AI22">
         <v>8.9</v>
       </c>
     </row>
-    <row r="23" spans="2:35">
+    <row r="23" spans="2:35" hidden="1">
       <c r="B23" t="s">
         <v>23</v>
       </c>
@@ -1392,11 +1366,8 @@
       <c r="AB24">
         <v>49</v>
       </c>
-      <c r="AC24">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="2:35">
+    </row>
+    <row r="25" spans="2:35" hidden="1">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -1440,7 +1411,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="26" spans="2:35">
+    <row r="26" spans="2:35" hidden="1">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -1466,7 +1437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="2:35">
+    <row r="27" spans="2:35" hidden="1">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1495,7 +1466,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="2:35">
+    <row r="28" spans="2:35" hidden="1">
       <c r="B28" t="s">
         <v>19</v>
       </c>
@@ -1536,7 +1507,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="2:35">
+    <row r="29" spans="2:35" hidden="1">
       <c r="B29" t="s">
         <v>19</v>
       </c>
@@ -1565,7 +1536,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="2:35">
+    <row r="30" spans="2:35" hidden="1">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -1609,7 +1580,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:35">
+    <row r="31" spans="2:35" hidden="1">
       <c r="B31" t="s">
         <v>18</v>
       </c>
@@ -1650,7 +1621,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="2:35">
+    <row r="32" spans="2:35" hidden="1">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -1676,7 +1647,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="2:31">
+    <row r="33" spans="2:31" hidden="1">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -1705,7 +1676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:31">
+    <row r="34" spans="2:31" hidden="1">
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1740,7 +1711,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="2:31">
+    <row r="35" spans="2:31" hidden="1">
       <c r="B35" t="s">
         <v>30</v>
       </c>
@@ -1763,7 +1734,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:31">
+    <row r="36" spans="2:31" hidden="1">
       <c r="B36" t="s">
         <v>30</v>
       </c>
@@ -1786,7 +1757,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:31">
+    <row r="37" spans="2:31" hidden="1">
       <c r="B37" t="s">
         <v>30</v>
       </c>
@@ -1809,7 +1780,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="2:31">
+    <row r="38" spans="2:31" hidden="1">
       <c r="B38" t="s">
         <v>30</v>
       </c>
@@ -1838,7 +1809,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="2:31">
+    <row r="39" spans="2:31" hidden="1">
       <c r="B39" t="s">
         <v>24</v>
       </c>
@@ -1904,11 +1875,8 @@
       <c r="AB40">
         <v>49</v>
       </c>
-      <c r="AC40">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="2:31">
+    </row>
+    <row r="41" spans="2:31" hidden="1">
       <c r="B41" t="s">
         <v>16</v>
       </c>
@@ -1943,7 +1911,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="2:31">
+    <row r="42" spans="2:31" hidden="1">
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -1978,7 +1946,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="2:31">
+    <row r="43" spans="2:31" hidden="1">
       <c r="B43" t="s">
         <v>30</v>
       </c>
@@ -2007,7 +1975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:31">
+    <row r="44" spans="2:31" hidden="1">
       <c r="B44" t="s">
         <v>30</v>
       </c>
@@ -2030,7 +1998,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="2:31">
+    <row r="45" spans="2:31" hidden="1">
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -2072,11 +2040,8 @@
       <c r="AB46">
         <v>49</v>
       </c>
-      <c r="AC46">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="2:31">
+    </row>
+    <row r="47" spans="2:31" hidden="1">
       <c r="B47" t="s">
         <v>30</v>
       </c>
@@ -2114,7 +2079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="2:31">
+    <row r="48" spans="2:31" hidden="1">
       <c r="B48" t="s">
         <v>30</v>
       </c>
@@ -2137,7 +2102,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:35">
+    <row r="49" spans="2:35" hidden="1">
       <c r="B49" t="s">
         <v>16</v>
       </c>
@@ -2172,7 +2137,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:35">
+    <row r="50" spans="2:35" hidden="1">
       <c r="B50" t="s">
         <v>18</v>
       </c>
@@ -2210,7 +2175,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="2:35">
+    <row r="51" spans="2:35" hidden="1">
       <c r="B51" t="s">
         <v>30</v>
       </c>
@@ -2236,7 +2201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:35">
+    <row r="52" spans="2:35" hidden="1">
       <c r="B52" t="s">
         <v>30</v>
       </c>
@@ -2259,7 +2224,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:35">
+    <row r="53" spans="2:35" hidden="1">
       <c r="B53" t="s">
         <v>30</v>
       </c>
@@ -2282,7 +2247,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="2:35">
+    <row r="54" spans="2:35" hidden="1">
       <c r="B54" t="s">
         <v>30</v>
       </c>
@@ -2323,7 +2288,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="55" spans="2:35">
+    <row r="55" spans="2:35" hidden="1">
       <c r="B55" t="s">
         <v>30</v>
       </c>
@@ -2346,7 +2311,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="2:35">
+    <row r="56" spans="2:35" hidden="1">
       <c r="B56" t="s">
         <v>30</v>
       </c>
@@ -2378,7 +2343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="2:35">
+    <row r="57" spans="2:35" hidden="1">
       <c r="B57" t="s">
         <v>18</v>
       </c>
@@ -2413,7 +2378,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="2:35">
+    <row r="58" spans="2:35" hidden="1">
       <c r="B58" t="s">
         <v>18</v>
       </c>
@@ -2448,7 +2413,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="2:35">
+    <row r="59" spans="2:35" hidden="1">
       <c r="B59" t="s">
         <v>30</v>
       </c>
@@ -2471,7 +2436,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="2:35">
+    <row r="60" spans="2:35" hidden="1">
       <c r="B60" t="s">
         <v>30</v>
       </c>
@@ -2509,7 +2474,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="2:35">
+    <row r="61" spans="2:35" hidden="1">
       <c r="B61" t="s">
         <v>18</v>
       </c>
@@ -2547,7 +2512,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="2:35">
+    <row r="62" spans="2:35" hidden="1">
       <c r="B62" t="s">
         <v>18</v>
       </c>
@@ -2585,7 +2550,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="2:35">
+    <row r="63" spans="2:35" hidden="1">
       <c r="B63" t="s">
         <v>18</v>
       </c>
@@ -2626,7 +2591,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="2:35">
+    <row r="64" spans="2:35" hidden="1">
       <c r="B64" t="s">
         <v>30</v>
       </c>
@@ -2649,7 +2614,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="2:29">
+    <row r="65" spans="2:29" hidden="1">
       <c r="B65" t="s">
         <v>30</v>
       </c>
@@ -2672,7 +2637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="2:29">
+    <row r="66" spans="2:29" hidden="1">
       <c r="B66" t="s">
         <v>18</v>
       </c>
@@ -2707,7 +2672,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="2:29">
+    <row r="67" spans="2:29" hidden="1">
       <c r="B67" t="s">
         <v>24</v>
       </c>
@@ -2749,11 +2714,8 @@
       <c r="AB68">
         <v>49</v>
       </c>
-      <c r="AC68">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="2:29">
+    </row>
+    <row r="69" spans="2:29" hidden="1">
       <c r="B69" t="s">
         <v>16</v>
       </c>
@@ -2788,7 +2750,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="2:29">
+    <row r="70" spans="2:29" hidden="1">
       <c r="B70" t="s">
         <v>16</v>
       </c>
@@ -2823,7 +2785,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="2:29">
+    <row r="71" spans="2:29" hidden="1">
       <c r="B71" t="s">
         <v>16</v>
       </c>
@@ -2858,7 +2820,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="2:29">
+    <row r="72" spans="2:29" hidden="1">
       <c r="B72" t="s">
         <v>24</v>
       </c>
@@ -2930,11 +2892,8 @@
       <c r="AB73">
         <v>49</v>
       </c>
-      <c r="AC73">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="2:29">
+    </row>
+    <row r="74" spans="2:29" hidden="1">
       <c r="B74" t="s">
         <v>16</v>
       </c>
@@ -2969,7 +2928,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="2:29">
+    <row r="75" spans="2:29" hidden="1">
       <c r="B75" t="s">
         <v>16</v>
       </c>
@@ -3004,7 +2963,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="2:29">
+    <row r="76" spans="2:29" hidden="1">
       <c r="B76" t="s">
         <v>16</v>
       </c>
@@ -3042,7 +3001,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="2:29">
+    <row r="77" spans="2:29" hidden="1">
       <c r="B77" t="s">
         <v>16</v>
       </c>
@@ -3077,7 +3036,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="2:29">
+    <row r="78" spans="2:29" hidden="1">
       <c r="B78" t="s">
         <v>30</v>
       </c>
@@ -3100,7 +3059,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="2:29">
+    <row r="79" spans="2:29" hidden="1">
       <c r="B79" t="s">
         <v>30</v>
       </c>
@@ -3126,7 +3085,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="2:29">
+    <row r="80" spans="2:29" hidden="1">
       <c r="B80" t="s">
         <v>24</v>
       </c>
@@ -3153,7 +3112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="2:35">
+    <row r="81" spans="2:35" hidden="1">
       <c r="B81" t="s">
         <v>30</v>
       </c>
@@ -3191,7 +3150,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="82" spans="2:35">
+    <row r="82" spans="2:35" hidden="1">
       <c r="B82" t="s">
         <v>30</v>
       </c>
@@ -3214,7 +3173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="2:35">
+    <row r="83" spans="2:35" hidden="1">
       <c r="B83" t="s">
         <v>18</v>
       </c>
@@ -3249,7 +3208,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="2:35">
+    <row r="84" spans="2:35" hidden="1">
       <c r="B84" t="s">
         <v>24</v>
       </c>
@@ -3284,7 +3243,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="85" spans="2:35">
+    <row r="85" spans="2:35" hidden="1">
       <c r="B85" t="s">
         <v>24</v>
       </c>
@@ -3319,7 +3278,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="2:35">
+    <row r="86" spans="2:35" hidden="1">
       <c r="B86" t="s">
         <v>24</v>
       </c>
@@ -3357,7 +3316,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="2:35">
+    <row r="87" spans="2:35" hidden="1">
       <c r="B87" t="s">
         <v>24</v>
       </c>
@@ -3411,9 +3370,6 @@
       <c r="AB88">
         <v>49</v>
       </c>
-      <c r="AC88">
-        <v>98</v>
-      </c>
     </row>
     <row r="89" spans="2:35">
       <c r="B89" t="s">
@@ -3437,9 +3393,6 @@
       <c r="AB89">
         <v>49</v>
       </c>
-      <c r="AC89">
-        <v>98</v>
-      </c>
       <c r="AI89">
         <v>4.0999999999999996</v>
       </c>
@@ -3475,9 +3428,6 @@
       <c r="AB90">
         <v>49</v>
       </c>
-      <c r="AC90">
-        <v>98</v>
-      </c>
     </row>
     <row r="91" spans="2:35">
       <c r="B91" t="s">
@@ -3513,9 +3463,6 @@
       <c r="AB91">
         <v>49</v>
       </c>
-      <c r="AC91">
-        <v>98</v>
-      </c>
     </row>
     <row r="92" spans="2:35">
       <c r="B92" t="s">
@@ -3542,11 +3489,8 @@
       <c r="AB92">
         <v>49</v>
       </c>
-      <c r="AC92">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="93" spans="2:35">
+    </row>
+    <row r="93" spans="2:35" hidden="1">
       <c r="B93" t="s">
         <v>16</v>
       </c>
@@ -3581,7 +3525,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="94" spans="2:35">
+    <row r="94" spans="2:35" hidden="1">
       <c r="B94" t="s">
         <v>30</v>
       </c>
@@ -3604,7 +3548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="2:35">
+    <row r="95" spans="2:35" hidden="1">
       <c r="B95" t="s">
         <v>30</v>
       </c>
@@ -3661,7 +3605,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="96" spans="2:35">
+    <row r="96" spans="2:35" hidden="1">
       <c r="B96" t="s">
         <v>18</v>
       </c>
@@ -3705,7 +3649,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="97" spans="2:34">
+    <row r="97" spans="2:34" hidden="1">
       <c r="B97" t="s">
         <v>18</v>
       </c>
@@ -3743,7 +3687,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="98" spans="2:34">
+    <row r="98" spans="2:34" hidden="1">
       <c r="B98" t="s">
         <v>17</v>
       </c>
@@ -3772,7 +3716,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="2:34">
+    <row r="99" spans="2:34" hidden="1">
       <c r="B99" t="s">
         <v>17</v>
       </c>
@@ -3795,7 +3739,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="2:34">
+    <row r="100" spans="2:34" hidden="1">
       <c r="B100" t="s">
         <v>14</v>
       </c>
@@ -3824,7 +3768,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="101" spans="2:34">
+    <row r="101" spans="2:34" hidden="1">
       <c r="B101" t="s">
         <v>15</v>
       </c>
@@ -3853,7 +3797,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="2:34">
+    <row r="102" spans="2:34" hidden="1">
       <c r="B102" t="s">
         <v>17</v>
       </c>
@@ -3895,9 +3839,6 @@
       <c r="AB103">
         <v>47</v>
       </c>
-      <c r="AC103">
-        <v>124</v>
-      </c>
     </row>
     <row r="104" spans="2:34">
       <c r="B104" t="s">
@@ -3927,11 +3868,8 @@
       <c r="AB104">
         <v>47</v>
       </c>
-      <c r="AC104">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="105" spans="2:34">
+    </row>
+    <row r="105" spans="2:34" hidden="1">
       <c r="B105" t="s">
         <v>23</v>
       </c>
@@ -4016,9 +3954,6 @@
       <c r="AB106">
         <v>49</v>
       </c>
-      <c r="AC106">
-        <v>111</v>
-      </c>
     </row>
     <row r="107" spans="2:34">
       <c r="B107" t="s">
@@ -4039,9 +3974,6 @@
       <c r="AB107">
         <v>47</v>
       </c>
-      <c r="AC107">
-        <v>124</v>
-      </c>
     </row>
     <row r="108" spans="2:34">
       <c r="B108" t="s">
@@ -4062,11 +3994,8 @@
       <c r="AB108">
         <v>47</v>
       </c>
-      <c r="AC108">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="109" spans="2:34">
+    </row>
+    <row r="109" spans="2:34" hidden="1">
       <c r="B109" t="s">
         <v>15</v>
       </c>
@@ -4108,11 +4037,8 @@
       <c r="AB110">
         <v>47</v>
       </c>
-      <c r="AC110">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="111" spans="2:34">
+    </row>
+    <row r="111" spans="2:34" hidden="1">
       <c r="B111" t="s">
         <v>14</v>
       </c>
@@ -4169,7 +4095,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="112" spans="2:34">
+    <row r="112" spans="2:34" hidden="1">
       <c r="B112" t="s">
         <v>23</v>
       </c>
@@ -4214,9 +4140,6 @@
       <c r="AB113">
         <v>47</v>
       </c>
-      <c r="AC113">
-        <v>124</v>
-      </c>
     </row>
     <row r="114" spans="2:35">
       <c r="B114" t="s">
@@ -4243,9 +4166,6 @@
       <c r="AB114">
         <v>47</v>
       </c>
-      <c r="AC114">
-        <v>124</v>
-      </c>
       <c r="AD114">
         <v>11</v>
       </c>
@@ -4272,11 +4192,8 @@
       <c r="AB115">
         <v>47</v>
       </c>
-      <c r="AC115">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="116" spans="2:35">
+    </row>
+    <row r="116" spans="2:35" hidden="1">
       <c r="B116" t="s">
         <v>17</v>
       </c>
@@ -4299,7 +4216,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="2:35">
+    <row r="117" spans="2:35" hidden="1">
       <c r="B117" t="s">
         <v>18</v>
       </c>
@@ -4390,9 +4307,6 @@
       <c r="AB118">
         <v>47</v>
       </c>
-      <c r="AC118">
-        <v>124</v>
-      </c>
     </row>
     <row r="119" spans="2:35">
       <c r="B119" t="s">
@@ -4413,9 +4327,6 @@
       <c r="AB119">
         <v>47</v>
       </c>
-      <c r="AC119">
-        <v>124</v>
-      </c>
     </row>
     <row r="120" spans="2:35">
       <c r="B120" t="s">
@@ -4436,9 +4347,6 @@
       <c r="AB120">
         <v>47</v>
       </c>
-      <c r="AC120">
-        <v>124</v>
-      </c>
     </row>
     <row r="121" spans="2:35">
       <c r="B121" t="s">
@@ -4462,9 +4370,6 @@
       <c r="AB121">
         <v>47</v>
       </c>
-      <c r="AC121">
-        <v>124</v>
-      </c>
       <c r="AD121">
         <v>12</v>
       </c>
@@ -4497,9 +4402,6 @@
       <c r="AB122">
         <v>47</v>
       </c>
-      <c r="AC122">
-        <v>124</v>
-      </c>
     </row>
     <row r="123" spans="2:35">
       <c r="B123" t="s">
@@ -4523,14 +4425,11 @@
       <c r="AB123">
         <v>47</v>
       </c>
-      <c r="AC123">
-        <v>124</v>
-      </c>
       <c r="AI123">
         <v>10.7</v>
       </c>
     </row>
-    <row r="124" spans="2:35">
+    <row r="124" spans="2:35" hidden="1">
       <c r="B124" t="s">
         <v>17</v>
       </c>
@@ -4572,9 +4471,6 @@
       <c r="AB125">
         <v>47</v>
       </c>
-      <c r="AC125">
-        <v>124</v>
-      </c>
     </row>
     <row r="126" spans="2:35">
       <c r="B126" t="s">
@@ -4595,9 +4491,6 @@
       <c r="AB126">
         <v>47</v>
       </c>
-      <c r="AC126">
-        <v>124</v>
-      </c>
       <c r="AE126">
         <v>5</v>
       </c>
@@ -4633,9 +4526,6 @@
       <c r="AB127">
         <v>47</v>
       </c>
-      <c r="AC127">
-        <v>124</v>
-      </c>
     </row>
     <row r="128" spans="2:35">
       <c r="B128" t="s">
@@ -4662,9 +4552,6 @@
       <c r="AB128">
         <v>47</v>
       </c>
-      <c r="AC128">
-        <v>124</v>
-      </c>
     </row>
     <row r="129" spans="2:35">
       <c r="B129" t="s">
@@ -4685,9 +4572,6 @@
       <c r="AB129">
         <v>47</v>
       </c>
-      <c r="AC129">
-        <v>124</v>
-      </c>
     </row>
     <row r="130" spans="2:35">
       <c r="B130" t="s">
@@ -4708,9 +4592,6 @@
       <c r="AB130">
         <v>47</v>
       </c>
-      <c r="AC130">
-        <v>124</v>
-      </c>
     </row>
     <row r="131" spans="2:35">
       <c r="B131" t="s">
@@ -4731,9 +4612,6 @@
       <c r="AB131">
         <v>47</v>
       </c>
-      <c r="AC131">
-        <v>124</v>
-      </c>
     </row>
     <row r="132" spans="2:35">
       <c r="B132" t="s">
@@ -4754,11 +4632,8 @@
       <c r="AB132">
         <v>47</v>
       </c>
-      <c r="AC132">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="133" spans="2:35">
+    </row>
+    <row r="133" spans="2:35" hidden="1">
       <c r="B133" t="s">
         <v>15</v>
       </c>
@@ -4809,9 +4684,6 @@
       <c r="AB134">
         <v>47</v>
       </c>
-      <c r="AC134">
-        <v>124</v>
-      </c>
     </row>
     <row r="135" spans="2:35">
       <c r="B135" t="s">
@@ -4838,9 +4710,6 @@
       <c r="AB135">
         <v>47</v>
       </c>
-      <c r="AC135">
-        <v>124</v>
-      </c>
       <c r="AD135">
         <v>1</v>
       </c>
@@ -4873,9 +4742,6 @@
       <c r="AB136">
         <v>47</v>
       </c>
-      <c r="AC136">
-        <v>124</v>
-      </c>
     </row>
     <row r="137" spans="2:35">
       <c r="B137" t="s">
@@ -4896,9 +4762,6 @@
       <c r="AB137">
         <v>47</v>
       </c>
-      <c r="AC137">
-        <v>124</v>
-      </c>
     </row>
     <row r="138" spans="2:35">
       <c r="B138" t="s">
@@ -4919,11 +4782,8 @@
       <c r="AB138">
         <v>47</v>
       </c>
-      <c r="AC138">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="139" spans="2:35">
+    </row>
+    <row r="139" spans="2:35" hidden="1">
       <c r="B139" t="s">
         <v>14</v>
       </c>
@@ -4949,7 +4809,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="2:35">
+    <row r="140" spans="2:35" hidden="1">
       <c r="B140" t="s">
         <v>25</v>
       </c>
@@ -5000,11 +4860,8 @@
       <c r="AB141">
         <v>49</v>
       </c>
-      <c r="AC141">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="142" spans="2:35">
+    </row>
+    <row r="142" spans="2:35" hidden="1">
       <c r="B142" t="s">
         <v>19</v>
       </c>
@@ -5050,9 +4907,6 @@
       <c r="AB143">
         <v>47</v>
       </c>
-      <c r="AC143">
-        <v>124</v>
-      </c>
     </row>
     <row r="144" spans="2:35">
       <c r="B144" t="s">
@@ -5082,9 +4936,6 @@
       <c r="AB144">
         <v>47</v>
       </c>
-      <c r="AC144">
-        <v>124</v>
-      </c>
     </row>
     <row r="145" spans="2:35">
       <c r="B145" t="s">
@@ -5121,9 +4972,6 @@
       <c r="AB145">
         <v>47</v>
       </c>
-      <c r="AC145">
-        <v>124</v>
-      </c>
       <c r="AD145">
         <v>1</v>
       </c>
@@ -5140,7 +4988,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="146" spans="2:35">
+    <row r="146" spans="2:35" hidden="1">
       <c r="B146" t="s">
         <v>32</v>
       </c>
@@ -5169,7 +5017,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="2:35">
+    <row r="147" spans="2:35" hidden="1">
       <c r="B147" t="s">
         <v>32</v>
       </c>
@@ -5198,7 +5046,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="2:35">
+    <row r="148" spans="2:35" hidden="1">
       <c r="B148" t="s">
         <v>32</v>
       </c>
@@ -5221,7 +5069,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="149" spans="2:35">
+    <row r="149" spans="2:35" hidden="1">
       <c r="B149" t="s">
         <v>32</v>
       </c>
@@ -5244,7 +5092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="2:35">
+    <row r="150" spans="2:35" hidden="1">
       <c r="B150" t="s">
         <v>32</v>
       </c>
@@ -5267,7 +5115,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="2:35">
+    <row r="151" spans="2:35" hidden="1">
       <c r="B151" t="s">
         <v>32</v>
       </c>
@@ -5290,7 +5138,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="152" spans="2:35">
+    <row r="152" spans="2:35" hidden="1">
       <c r="B152" t="s">
         <v>32</v>
       </c>
@@ -5313,7 +5161,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="153" spans="2:35">
+    <row r="153" spans="2:35" hidden="1">
       <c r="B153" t="s">
         <v>32</v>
       </c>
@@ -5342,7 +5190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="2:35">
+    <row r="154" spans="2:35" hidden="1">
       <c r="B154" t="s">
         <v>19</v>
       </c>
@@ -5368,7 +5216,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="155" spans="2:35">
+    <row r="155" spans="2:35" hidden="1">
       <c r="B155" t="s">
         <v>19</v>
       </c>
@@ -5391,7 +5239,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="156" spans="2:35">
+    <row r="156" spans="2:35" hidden="1">
       <c r="B156" t="s">
         <v>32</v>
       </c>
@@ -5417,7 +5265,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="157" spans="2:35">
+    <row r="157" spans="2:35" hidden="1">
       <c r="B157" t="s">
         <v>32</v>
       </c>
@@ -5443,7 +5291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="158" spans="2:35">
+    <row r="158" spans="2:35" hidden="1">
       <c r="B158" t="s">
         <v>25</v>
       </c>
@@ -5479,7 +5327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:35">
+    <row r="159" spans="2:35" hidden="1">
       <c r="B159" t="s">
         <v>19</v>
       </c>
@@ -5542,11 +5390,8 @@
       <c r="AB160">
         <v>49</v>
       </c>
-      <c r="AC160">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="161" spans="2:34">
+    </row>
+    <row r="161" spans="2:34" hidden="1">
       <c r="B161" t="s">
         <v>32</v>
       </c>
@@ -5569,7 +5414,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="162" spans="2:34">
+    <row r="162" spans="2:34" hidden="1">
       <c r="B162" t="s">
         <v>32</v>
       </c>
@@ -5592,7 +5437,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="2:34">
+    <row r="163" spans="2:34" hidden="1">
       <c r="B163" t="s">
         <v>32</v>
       </c>
@@ -5615,7 +5460,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="164" spans="2:34">
+    <row r="164" spans="2:34" hidden="1">
       <c r="B164" t="s">
         <v>32</v>
       </c>
@@ -5647,7 +5492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="2:34">
+    <row r="165" spans="2:34" hidden="1">
       <c r="B165" t="s">
         <v>17</v>
       </c>
@@ -5698,7 +5543,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="166" spans="2:34">
+    <row r="166" spans="2:34" hidden="1">
       <c r="B166" t="s">
         <v>17</v>
       </c>
@@ -5721,7 +5566,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="167" spans="2:34">
+    <row r="167" spans="2:34" hidden="1">
       <c r="B167" t="s">
         <v>14</v>
       </c>
@@ -5747,7 +5592,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="168" spans="2:34">
+    <row r="168" spans="2:34" hidden="1">
       <c r="B168" t="s">
         <v>14</v>
       </c>
@@ -5795,11 +5640,8 @@
       <c r="AB169">
         <v>49</v>
       </c>
-      <c r="AC169">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="170" spans="2:34">
+    </row>
+    <row r="170" spans="2:34" hidden="1">
       <c r="B170" t="s">
         <v>32</v>
       </c>
@@ -5828,7 +5670,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="171" spans="2:34">
+    <row r="171" spans="2:34" hidden="1">
       <c r="B171" t="s">
         <v>25</v>
       </c>
@@ -5851,7 +5693,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="172" spans="2:34">
+    <row r="172" spans="2:34" hidden="1">
       <c r="B172" t="s">
         <v>15</v>
       </c>
@@ -5908,7 +5750,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="173" spans="2:34">
+    <row r="173" spans="2:34" hidden="1">
       <c r="B173" t="s">
         <v>25</v>
       </c>
@@ -5956,11 +5798,8 @@
       <c r="AB174">
         <v>49</v>
       </c>
-      <c r="AC174">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="175" spans="2:34">
+    </row>
+    <row r="175" spans="2:34" hidden="1">
       <c r="B175" t="s">
         <v>32</v>
       </c>
@@ -5989,7 +5828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="2:34">
+    <row r="176" spans="2:34" hidden="1">
       <c r="B176" t="s">
         <v>32</v>
       </c>
@@ -6015,7 +5854,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="177" spans="2:34">
+    <row r="177" spans="2:34" hidden="1">
       <c r="B177" t="s">
         <v>32</v>
       </c>
@@ -6041,7 +5880,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="178" spans="2:34">
+    <row r="178" spans="2:34" hidden="1">
       <c r="B178" t="s">
         <v>32</v>
       </c>
@@ -6064,7 +5903,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="179" spans="2:34">
+    <row r="179" spans="2:34" hidden="1">
       <c r="B179" t="s">
         <v>14</v>
       </c>
@@ -6090,7 +5929,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="2:34">
+    <row r="180" spans="2:34" hidden="1">
       <c r="B180" t="s">
         <v>25</v>
       </c>
@@ -6144,11 +5983,8 @@
       <c r="AB181">
         <v>49</v>
       </c>
-      <c r="AC181">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="182" spans="2:34">
+    </row>
+    <row r="182" spans="2:34" hidden="1">
       <c r="B182" t="s">
         <v>19</v>
       </c>
@@ -6205,7 +6041,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="183" spans="2:34">
+    <row r="183" spans="2:34" hidden="1">
       <c r="B183" t="s">
         <v>23</v>
       </c>
@@ -6253,11 +6089,8 @@
       <c r="AB184">
         <v>49</v>
       </c>
-      <c r="AC184">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="185" spans="2:34">
+    </row>
+    <row r="185" spans="2:34" hidden="1">
       <c r="B185" t="s">
         <v>15</v>
       </c>
@@ -6280,7 +6113,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="186" spans="2:34">
+    <row r="186" spans="2:34" hidden="1">
       <c r="B186" t="s">
         <v>23</v>
       </c>
@@ -6360,11 +6193,8 @@
       <c r="AB187">
         <v>49</v>
       </c>
-      <c r="AC187">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="188" spans="2:34">
+    </row>
+    <row r="188" spans="2:34" hidden="1">
       <c r="B188" t="s">
         <v>15</v>
       </c>
@@ -6412,11 +6242,8 @@
       <c r="AB189">
         <v>49</v>
       </c>
-      <c r="AC189">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="190" spans="2:34">
+    </row>
+    <row r="190" spans="2:34" hidden="1">
       <c r="B190" t="s">
         <v>15</v>
       </c>
@@ -6439,7 +6266,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="191" spans="2:34">
+    <row r="191" spans="2:34" hidden="1">
       <c r="B191" t="s">
         <v>15</v>
       </c>
@@ -6462,7 +6289,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="192" spans="2:34">
+    <row r="192" spans="2:34" hidden="1">
       <c r="B192" t="s">
         <v>15</v>
       </c>
@@ -6485,7 +6312,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="193" spans="2:35">
+    <row r="193" spans="2:35" hidden="1">
       <c r="B193" t="s">
         <v>14</v>
       </c>
@@ -6511,7 +6338,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="194" spans="2:35">
+    <row r="194" spans="2:35" hidden="1">
       <c r="B194" t="s">
         <v>16</v>
       </c>
@@ -6553,11 +6380,8 @@
       <c r="AB195">
         <v>49</v>
       </c>
-      <c r="AC195">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="196" spans="2:35">
+    </row>
+    <row r="196" spans="2:35" hidden="1">
       <c r="B196" t="s">
         <v>17</v>
       </c>
@@ -6580,7 +6404,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="197" spans="2:35">
+    <row r="197" spans="2:35" hidden="1">
       <c r="B197" t="s">
         <v>17</v>
       </c>
@@ -6622,11 +6446,8 @@
       <c r="AB198">
         <v>49</v>
       </c>
-      <c r="AC198">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="199" spans="2:35">
+    </row>
+    <row r="199" spans="2:35" hidden="1">
       <c r="B199" t="s">
         <v>16</v>
       </c>
@@ -6649,7 +6470,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="200" spans="2:35">
+    <row r="200" spans="2:35" hidden="1">
       <c r="B200" t="s">
         <v>32</v>
       </c>
@@ -6687,7 +6508,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="201" spans="2:35">
+    <row r="201" spans="2:35" hidden="1">
       <c r="B201" t="s">
         <v>24</v>
       </c>
@@ -6713,7 +6534,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="202" spans="2:35">
+    <row r="202" spans="2:35" hidden="1">
       <c r="B202" t="s">
         <v>17</v>
       </c>
@@ -6736,7 +6557,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="203" spans="2:35">
+    <row r="203" spans="2:35" hidden="1">
       <c r="B203" t="s">
         <v>17</v>
       </c>
@@ -6759,7 +6580,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="204" spans="2:35">
+    <row r="204" spans="2:35" hidden="1">
       <c r="B204" t="s">
         <v>17</v>
       </c>
@@ -6782,7 +6603,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="205" spans="2:35">
+    <row r="205" spans="2:35" hidden="1">
       <c r="B205" t="s">
         <v>14</v>
       </c>
@@ -6805,7 +6626,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="206" spans="2:35">
+    <row r="206" spans="2:35" hidden="1">
       <c r="B206" t="s">
         <v>16</v>
       </c>
@@ -6828,7 +6649,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="207" spans="2:35">
+    <row r="207" spans="2:35" hidden="1">
       <c r="B207" t="s">
         <v>16</v>
       </c>
@@ -6851,7 +6672,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="208" spans="2:35">
+    <row r="208" spans="2:35" hidden="1">
       <c r="B208" t="s">
         <v>16</v>
       </c>
@@ -6874,7 +6695,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="209" spans="2:35">
+    <row r="209" spans="2:35" hidden="1">
       <c r="B209" t="s">
         <v>23</v>
       </c>
@@ -6900,7 +6721,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="210" spans="2:35">
+    <row r="210" spans="2:35" hidden="1">
       <c r="B210" t="s">
         <v>18</v>
       </c>
@@ -6960,11 +6781,8 @@
       <c r="AB211">
         <v>49</v>
       </c>
-      <c r="AC211">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="212" spans="2:35">
+    </row>
+    <row r="212" spans="2:35" hidden="1">
       <c r="B212" t="s">
         <v>32</v>
       </c>
@@ -6987,7 +6805,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="213" spans="2:35">
+    <row r="213" spans="2:35" hidden="1">
       <c r="B213" t="s">
         <v>32</v>
       </c>
@@ -7019,7 +6837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="2:35">
+    <row r="214" spans="2:35" hidden="1">
       <c r="B214" t="s">
         <v>32</v>
       </c>
@@ -7045,7 +6863,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="215" spans="2:35">
+    <row r="215" spans="2:35" hidden="1">
       <c r="B215" t="s">
         <v>32</v>
       </c>
@@ -7105,14 +6923,11 @@
       <c r="AB216">
         <v>49</v>
       </c>
-      <c r="AC216">
-        <v>111</v>
-      </c>
       <c r="AI216">
         <v>7.6</v>
       </c>
     </row>
-    <row r="217" spans="2:35">
+    <row r="217" spans="2:35" hidden="1">
       <c r="B217" t="s">
         <v>14</v>
       </c>
@@ -7135,7 +6950,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="218" spans="2:35">
+    <row r="218" spans="2:35" hidden="1">
       <c r="B218" t="s">
         <v>23</v>
       </c>
@@ -7155,7 +6970,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="219" spans="2:35">
+    <row r="219" spans="2:35" hidden="1">
       <c r="B219" t="s">
         <v>32</v>
       </c>
@@ -7181,7 +6996,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="220" spans="2:35">
+    <row r="220" spans="2:35" hidden="1">
       <c r="B220" t="s">
         <v>32</v>
       </c>
@@ -7223,11 +7038,8 @@
       <c r="AB221">
         <v>49</v>
       </c>
-      <c r="AC221">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="222" spans="2:35">
+    </row>
+    <row r="222" spans="2:35" hidden="1">
       <c r="B222" t="s">
         <v>23</v>
       </c>
@@ -7290,11 +7102,8 @@
       <c r="AB223">
         <v>49</v>
       </c>
-      <c r="AC223">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="224" spans="2:35">
+    </row>
+    <row r="224" spans="2:35" hidden="1">
       <c r="B224" t="s">
         <v>15</v>
       </c>
@@ -7317,7 +7126,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="225" spans="2:35">
+    <row r="225" spans="2:35" hidden="1">
       <c r="B225" t="s">
         <v>18</v>
       </c>
@@ -7343,7 +7152,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="226" spans="2:35">
+    <row r="226" spans="2:35" hidden="1">
       <c r="B226" t="s">
         <v>16</v>
       </c>
@@ -7366,7 +7175,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="227" spans="2:35">
+    <row r="227" spans="2:35" hidden="1">
       <c r="B227" t="s">
         <v>17</v>
       </c>
@@ -7389,7 +7198,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="228" spans="2:35">
+    <row r="228" spans="2:35" hidden="1">
       <c r="B228" t="s">
         <v>32</v>
       </c>
@@ -7415,7 +7224,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="229" spans="2:35">
+    <row r="229" spans="2:35" hidden="1">
       <c r="B229" t="s">
         <v>32</v>
       </c>
@@ -7438,7 +7247,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="230" spans="2:35">
+    <row r="230" spans="2:35" hidden="1">
       <c r="B230" t="s">
         <v>32</v>
       </c>
@@ -7473,7 +7282,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="231" spans="2:35">
+    <row r="231" spans="2:35" hidden="1">
       <c r="B231" t="s">
         <v>32</v>
       </c>
@@ -7508,7 +7317,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="232" spans="2:35">
+    <row r="232" spans="2:35" hidden="1">
       <c r="B232" t="s">
         <v>17</v>
       </c>
@@ -7531,7 +7340,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="233" spans="2:35">
+    <row r="233" spans="2:35" hidden="1">
       <c r="B233" t="s">
         <v>16</v>
       </c>
@@ -7554,7 +7363,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="234" spans="2:35">
+    <row r="234" spans="2:35" hidden="1">
       <c r="B234" t="s">
         <v>32</v>
       </c>
@@ -7577,7 +7386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="235" spans="2:35">
+    <row r="235" spans="2:35" hidden="1">
       <c r="B235" t="s">
         <v>32</v>
       </c>
@@ -7600,7 +7409,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="236" spans="2:35">
+    <row r="236" spans="2:35" hidden="1">
       <c r="B236" t="s">
         <v>23</v>
       </c>
@@ -7629,7 +7438,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="237" spans="2:35">
+    <row r="237" spans="2:35" hidden="1">
       <c r="B237" t="s">
         <v>24</v>
       </c>
@@ -7655,7 +7464,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="238" spans="2:35">
+    <row r="238" spans="2:35" hidden="1">
       <c r="B238" t="s">
         <v>17</v>
       </c>
@@ -7678,7 +7487,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="239" spans="2:35">
+    <row r="239" spans="2:35" hidden="1">
       <c r="B239" t="s">
         <v>23</v>
       </c>
@@ -7701,7 +7510,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="240" spans="2:35">
+    <row r="240" spans="2:35" hidden="1">
       <c r="B240" t="s">
         <v>32</v>
       </c>
@@ -7725,7 +7534,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="241" spans="2:34">
+    <row r="241" spans="2:34" hidden="1">
       <c r="B241" t="s">
         <v>23</v>
       </c>
@@ -7748,7 +7557,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="242" spans="2:34">
+    <row r="242" spans="2:34" hidden="1">
       <c r="B242" t="s">
         <v>14</v>
       </c>
@@ -7771,7 +7580,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="243" spans="2:34">
+    <row r="243" spans="2:34" hidden="1">
       <c r="B243" t="s">
         <v>32</v>
       </c>
@@ -7825,7 +7634,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="244" spans="2:34">
+    <row r="244" spans="2:34" hidden="1">
       <c r="B244" t="s">
         <v>14</v>
       </c>
@@ -7870,9 +7679,6 @@
       <c r="AB245">
         <v>47</v>
       </c>
-      <c r="AC245">
-        <v>124</v>
-      </c>
     </row>
     <row r="246" spans="2:34">
       <c r="B246" t="s">
@@ -7893,9 +7699,6 @@
       <c r="AB246">
         <v>49</v>
       </c>
-      <c r="AC246">
-        <v>111</v>
-      </c>
     </row>
     <row r="247" spans="2:34">
       <c r="B247" t="s">
@@ -7925,11 +7728,8 @@
       <c r="AB247">
         <v>47</v>
       </c>
-      <c r="AC247">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="248" spans="2:34">
+    </row>
+    <row r="248" spans="2:34" hidden="1">
       <c r="B248" t="s">
         <v>17</v>
       </c>
@@ -7952,7 +7752,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="249" spans="2:34">
+    <row r="249" spans="2:34" hidden="1">
       <c r="B249" t="s">
         <v>15</v>
       </c>
@@ -8009,9 +7809,6 @@
       <c r="AB250">
         <v>49</v>
       </c>
-      <c r="AC250">
-        <v>98</v>
-      </c>
     </row>
     <row r="251" spans="2:34">
       <c r="B251" t="s">
@@ -8035,9 +7832,6 @@
       <c r="AB251">
         <v>47</v>
       </c>
-      <c r="AC251">
-        <v>124</v>
-      </c>
     </row>
     <row r="252" spans="2:34">
       <c r="B252" t="s">
@@ -8058,9 +7852,6 @@
       <c r="AB252">
         <v>47</v>
       </c>
-      <c r="AC252">
-        <v>124</v>
-      </c>
     </row>
     <row r="253" spans="2:34">
       <c r="B253" t="s">
@@ -8081,9 +7872,6 @@
       <c r="AB253">
         <v>47</v>
       </c>
-      <c r="AC253">
-        <v>124</v>
-      </c>
     </row>
     <row r="254" spans="2:34">
       <c r="B254" t="s">
@@ -8104,9 +7892,6 @@
       <c r="AB254">
         <v>47</v>
       </c>
-      <c r="AC254">
-        <v>124</v>
-      </c>
     </row>
     <row r="255" spans="2:34">
       <c r="B255" t="s">
@@ -8136,11 +7921,8 @@
       <c r="AB255">
         <v>49</v>
       </c>
-      <c r="AC255">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="256" spans="2:34">
+    </row>
+    <row r="256" spans="2:34" hidden="1">
       <c r="B256" t="s">
         <v>17</v>
       </c>
@@ -8163,7 +7945,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="257" spans="2:31">
+    <row r="257" spans="2:31" hidden="1">
       <c r="B257" t="s">
         <v>15</v>
       </c>
@@ -8205,9 +7987,6 @@
       <c r="AB258">
         <v>47</v>
       </c>
-      <c r="AC258">
-        <v>124</v>
-      </c>
     </row>
     <row r="259" spans="2:31">
       <c r="B259" t="s">
@@ -8231,9 +8010,6 @@
       <c r="AB259">
         <v>47</v>
       </c>
-      <c r="AC259">
-        <v>124</v>
-      </c>
     </row>
     <row r="260" spans="2:31">
       <c r="B260" t="s">
@@ -8257,9 +8033,6 @@
       <c r="AB260">
         <v>47</v>
       </c>
-      <c r="AC260">
-        <v>124</v>
-      </c>
       <c r="AD260">
         <v>9</v>
       </c>
@@ -8267,7 +8040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="2:31">
+    <row r="261" spans="2:31" hidden="1">
       <c r="B261" t="s">
         <v>15</v>
       </c>
@@ -8309,9 +8082,6 @@
       <c r="AB262">
         <v>47</v>
       </c>
-      <c r="AC262">
-        <v>124</v>
-      </c>
     </row>
     <row r="263" spans="2:31">
       <c r="B263" t="s">
@@ -8332,11 +8102,8 @@
       <c r="AB263">
         <v>47</v>
       </c>
-      <c r="AC263">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="264" spans="2:31">
+    </row>
+    <row r="264" spans="2:31" hidden="1">
       <c r="B264" t="s">
         <v>14</v>
       </c>
@@ -8387,9 +8154,6 @@
       <c r="AB265">
         <v>47</v>
       </c>
-      <c r="AC265">
-        <v>124</v>
-      </c>
     </row>
     <row r="266" spans="2:31">
       <c r="B266" t="s">
@@ -8410,9 +8174,6 @@
       <c r="AB266">
         <v>47</v>
       </c>
-      <c r="AC266">
-        <v>124</v>
-      </c>
     </row>
     <row r="267" spans="2:31">
       <c r="B267" t="s">
@@ -8433,11 +8194,8 @@
       <c r="AB267">
         <v>49</v>
       </c>
-      <c r="AC267">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="268" spans="2:31">
+    </row>
+    <row r="268" spans="2:31" hidden="1">
       <c r="B268" t="s">
         <v>18</v>
       </c>
@@ -8460,7 +8218,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="269" spans="2:31">
+    <row r="269" spans="2:31" hidden="1">
       <c r="B269" t="s">
         <v>18</v>
       </c>
@@ -8502,11 +8260,8 @@
       <c r="AB270">
         <v>47</v>
       </c>
-      <c r="AC270">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="271" spans="2:31">
+    </row>
+    <row r="271" spans="2:31" hidden="1">
       <c r="B271" t="s">
         <v>24</v>
       </c>
@@ -8566,11 +8321,8 @@
       <c r="AB272">
         <v>47</v>
       </c>
-      <c r="AC272">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="273" spans="2:35">
+    </row>
+    <row r="273" spans="2:35" hidden="1">
       <c r="B273" t="s">
         <v>24</v>
       </c>
@@ -8612,14 +8364,11 @@
       <c r="AB274">
         <v>47</v>
       </c>
-      <c r="AC274">
-        <v>124</v>
-      </c>
       <c r="AE274">
         <v>8</v>
       </c>
     </row>
-    <row r="275" spans="2:35">
+    <row r="275" spans="2:35" hidden="1">
       <c r="B275" t="s">
         <v>18</v>
       </c>
@@ -8642,7 +8391,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="276" spans="2:35">
+    <row r="276" spans="2:35" hidden="1">
       <c r="B276" t="s">
         <v>16</v>
       </c>
@@ -8668,7 +8417,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="277" spans="2:35">
+    <row r="277" spans="2:35" hidden="1">
       <c r="B277" t="s">
         <v>14</v>
       </c>
@@ -8713,9 +8462,6 @@
       <c r="AB278">
         <v>47</v>
       </c>
-      <c r="AC278">
-        <v>124</v>
-      </c>
     </row>
     <row r="279" spans="2:35">
       <c r="B279" t="s">
@@ -8736,11 +8482,8 @@
       <c r="AB279">
         <v>49</v>
       </c>
-      <c r="AC279">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="280" spans="2:35">
+    </row>
+    <row r="280" spans="2:35" hidden="1">
       <c r="B280" t="s">
         <v>24</v>
       </c>
@@ -8770,7 +8513,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="281" spans="2:35">
+    <row r="281" spans="2:35" hidden="1">
       <c r="B281" t="s">
         <v>23</v>
       </c>
@@ -8815,9 +8558,6 @@
       <c r="AB282">
         <v>47</v>
       </c>
-      <c r="AC282">
-        <v>124</v>
-      </c>
     </row>
     <row r="283" spans="2:35">
       <c r="B283" t="s">
@@ -8847,9 +8587,6 @@
       <c r="AB283">
         <v>47</v>
       </c>
-      <c r="AC283">
-        <v>124</v>
-      </c>
     </row>
     <row r="284" spans="2:35">
       <c r="B284" t="s">
@@ -8870,9 +8607,6 @@
       <c r="AB284">
         <v>47</v>
       </c>
-      <c r="AC284">
-        <v>124</v>
-      </c>
       <c r="AI284">
         <v>5.5</v>
       </c>
@@ -8896,9 +8630,6 @@
       <c r="AB285">
         <v>47</v>
       </c>
-      <c r="AC285">
-        <v>124</v>
-      </c>
     </row>
     <row r="286" spans="2:35">
       <c r="B286" t="s">
@@ -8919,9 +8650,6 @@
       <c r="AB286">
         <v>47</v>
       </c>
-      <c r="AC286">
-        <v>124</v>
-      </c>
       <c r="AD286">
         <v>1</v>
       </c>
@@ -8960,11 +8688,8 @@
       <c r="AB287">
         <v>47</v>
       </c>
-      <c r="AC287">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="288" spans="2:35">
+    </row>
+    <row r="288" spans="2:35" hidden="1">
       <c r="B288" t="s">
         <v>18</v>
       </c>
@@ -8987,7 +8712,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="289" spans="2:35">
+    <row r="289" spans="2:35" hidden="1">
       <c r="B289" t="s">
         <v>14</v>
       </c>
@@ -9032,11 +8757,8 @@
       <c r="AB290">
         <v>47</v>
       </c>
-      <c r="AC290">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="291" spans="2:35">
+    </row>
+    <row r="291" spans="2:35" hidden="1">
       <c r="B291" t="s">
         <v>16</v>
       </c>
@@ -9081,9 +8803,6 @@
       <c r="AB292">
         <v>47</v>
       </c>
-      <c r="AC292">
-        <v>124</v>
-      </c>
     </row>
     <row r="293" spans="2:35">
       <c r="B293" t="s">
@@ -9104,9 +8823,6 @@
       <c r="AB293">
         <v>47</v>
       </c>
-      <c r="AC293">
-        <v>124</v>
-      </c>
     </row>
     <row r="294" spans="2:35">
       <c r="B294" t="s">
@@ -9128,11 +8844,8 @@
       <c r="AB294">
         <v>47</v>
       </c>
-      <c r="AC294">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="295" spans="2:35">
+    </row>
+    <row r="295" spans="2:35" hidden="1">
       <c r="B295" t="s">
         <v>24</v>
       </c>
@@ -9180,9 +8893,6 @@
       <c r="AB296">
         <v>47</v>
       </c>
-      <c r="AC296">
-        <v>124</v>
-      </c>
     </row>
     <row r="297" spans="2:35">
       <c r="B297" t="s">
@@ -9206,9 +8916,6 @@
       <c r="AB297">
         <v>47</v>
       </c>
-      <c r="AC297">
-        <v>124</v>
-      </c>
       <c r="AE297">
         <v>4</v>
       </c>
@@ -9219,7 +8926,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="298" spans="2:35">
+    <row r="298" spans="2:35" hidden="1">
       <c r="B298" t="s">
         <v>14</v>
       </c>
@@ -9264,9 +8971,6 @@
       <c r="AB299">
         <v>49</v>
       </c>
-      <c r="AC299">
-        <v>98</v>
-      </c>
     </row>
     <row r="300" spans="2:35">
       <c r="B300" t="s">
@@ -9287,11 +8991,8 @@
       <c r="AB300">
         <v>47</v>
       </c>
-      <c r="AC300">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="301" spans="2:35">
+    </row>
+    <row r="301" spans="2:35" hidden="1">
       <c r="B301" t="s">
         <v>19</v>
       </c>
@@ -9334,9 +9035,6 @@
       <c r="AB302">
         <v>49</v>
       </c>
-      <c r="AC302">
-        <v>98</v>
-      </c>
     </row>
     <row r="303" spans="2:35">
       <c r="B303" t="s">
@@ -9360,11 +9058,8 @@
       <c r="AB303">
         <v>49</v>
       </c>
-      <c r="AC303">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="304" spans="2:35">
+    </row>
+    <row r="304" spans="2:35" hidden="1">
       <c r="B304" t="s">
         <v>19</v>
       </c>
@@ -9387,7 +9082,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="305" spans="2:29">
+    <row r="305" spans="2:29" hidden="1">
       <c r="B305" t="s">
         <v>19</v>
       </c>
@@ -9410,7 +9105,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="306" spans="2:29">
+    <row r="306" spans="2:29" hidden="1">
       <c r="B306" t="s">
         <v>25</v>
       </c>
@@ -9439,7 +9134,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="307" spans="2:29">
+    <row r="307" spans="2:29" hidden="1">
       <c r="B307" t="s">
         <v>25</v>
       </c>
@@ -9495,9 +9190,6 @@
       <c r="AB308">
         <v>47</v>
       </c>
-      <c r="AC308">
-        <v>124</v>
-      </c>
     </row>
     <row r="309" spans="2:29">
       <c r="B309" t="s">
@@ -9518,9 +9210,6 @@
       <c r="AB309">
         <v>49</v>
       </c>
-      <c r="AC309">
-        <v>91</v>
-      </c>
     </row>
     <row r="310" spans="2:29">
       <c r="B310" t="s">
@@ -9544,11 +9233,8 @@
       <c r="AB310">
         <v>49</v>
       </c>
-      <c r="AC310">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="311" spans="2:29">
+    </row>
+    <row r="311" spans="2:29" hidden="1">
       <c r="B311" t="s">
         <v>18</v>
       </c>
@@ -9590,9 +9276,6 @@
       <c r="AB312">
         <v>47</v>
       </c>
-      <c r="AC312">
-        <v>124</v>
-      </c>
     </row>
     <row r="313" spans="2:29">
       <c r="B313" t="s">
@@ -9613,11 +9296,8 @@
       <c r="AB313">
         <v>47</v>
       </c>
-      <c r="AC313">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="314" spans="2:29">
+    </row>
+    <row r="314" spans="2:29" hidden="1">
       <c r="B314" t="s">
         <v>18</v>
       </c>
@@ -9640,7 +9320,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="315" spans="2:29">
+    <row r="315" spans="2:29" hidden="1">
       <c r="B315" t="s">
         <v>18</v>
       </c>
@@ -9663,7 +9343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="316" spans="2:29">
+    <row r="316" spans="2:29" hidden="1">
       <c r="B316" t="s">
         <v>25</v>
       </c>
@@ -9686,7 +9366,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="317" spans="2:29">
+    <row r="317" spans="2:29" hidden="1">
       <c r="B317" t="s">
         <v>14</v>
       </c>
@@ -9712,7 +9392,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="318" spans="2:29">
+    <row r="318" spans="2:29" hidden="1">
       <c r="B318" t="s">
         <v>17</v>
       </c>
@@ -9735,7 +9415,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="319" spans="2:29">
+    <row r="319" spans="2:29" hidden="1">
       <c r="B319" t="s">
         <v>18</v>
       </c>
@@ -9758,7 +9438,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="320" spans="2:29">
+    <row r="320" spans="2:29" hidden="1">
       <c r="B320" t="s">
         <v>19</v>
       </c>
@@ -9807,9 +9487,6 @@
       <c r="AB321">
         <v>49</v>
       </c>
-      <c r="AC321">
-        <v>91</v>
-      </c>
     </row>
     <row r="322" spans="2:34">
       <c r="B322" t="s">
@@ -9830,9 +9507,6 @@
       <c r="AB322">
         <v>47</v>
       </c>
-      <c r="AC322">
-        <v>124</v>
-      </c>
     </row>
     <row r="323" spans="2:34">
       <c r="B323" t="s">
@@ -9853,11 +9527,8 @@
       <c r="AB323">
         <v>47</v>
       </c>
-      <c r="AC323">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="324" spans="2:34">
+    </row>
+    <row r="324" spans="2:34" hidden="1">
       <c r="B324" t="s">
         <v>25</v>
       </c>
@@ -9905,11 +9576,8 @@
       <c r="AB325">
         <v>47</v>
       </c>
-      <c r="AC325">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="326" spans="2:34">
+    </row>
+    <row r="326" spans="2:34" hidden="1">
       <c r="B326" t="s">
         <v>19</v>
       </c>
@@ -9935,7 +9603,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="327" spans="2:34">
+    <row r="327" spans="2:34" hidden="1">
       <c r="B327" t="s">
         <v>19</v>
       </c>
@@ -9959,7 +9627,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="328" spans="2:34">
+    <row r="328" spans="2:34" hidden="1">
       <c r="B328" t="s">
         <v>18</v>
       </c>
@@ -9988,7 +9656,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="329" spans="2:34">
+    <row r="329" spans="2:34" hidden="1">
       <c r="B329" t="s">
         <v>17</v>
       </c>
@@ -10014,7 +9682,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="330" spans="2:34">
+    <row r="330" spans="2:34" hidden="1">
       <c r="B330" t="s">
         <v>25</v>
       </c>
@@ -10037,7 +9705,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="331" spans="2:34">
+    <row r="331" spans="2:34" hidden="1">
       <c r="B331" t="s">
         <v>14</v>
       </c>
@@ -10066,7 +9734,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="332" spans="2:34">
+    <row r="332" spans="2:34" hidden="1">
       <c r="B332" t="s">
         <v>25</v>
       </c>
@@ -10123,9 +9791,6 @@
       <c r="AB333">
         <v>49</v>
       </c>
-      <c r="AC333">
-        <v>91</v>
-      </c>
     </row>
     <row r="334" spans="2:34">
       <c r="B334" t="s">
@@ -10152,9 +9817,6 @@
       <c r="AB334">
         <v>47</v>
       </c>
-      <c r="AC334">
-        <v>124</v>
-      </c>
     </row>
     <row r="335" spans="2:34">
       <c r="B335" t="s">
@@ -10175,9 +9837,6 @@
       <c r="AB335">
         <v>47</v>
       </c>
-      <c r="AC335">
-        <v>124</v>
-      </c>
     </row>
     <row r="336" spans="2:34">
       <c r="B336" t="s">
@@ -10223,9 +9882,6 @@
       <c r="AB336">
         <v>47</v>
       </c>
-      <c r="AC336">
-        <v>124</v>
-      </c>
       <c r="AF336">
         <v>16</v>
       </c>
@@ -10236,7 +9892,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="337" spans="1:31">
+    <row r="337" spans="1:31" hidden="1">
       <c r="A337" t="s">
         <v>20</v>
       </c>
@@ -10277,7 +9933,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="338" spans="1:31">
+    <row r="338" spans="1:31" hidden="1">
       <c r="B338" t="s">
         <v>34</v>
       </c>
@@ -10306,7 +9962,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="339" spans="1:31">
+    <row r="339" spans="1:31" hidden="1">
       <c r="B339" t="s">
         <v>34</v>
       </c>
@@ -10329,7 +9985,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="340" spans="1:31">
+    <row r="340" spans="1:31" hidden="1">
       <c r="B340" t="s">
         <v>34</v>
       </c>
@@ -10367,7 +10023,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="341" spans="1:31">
+    <row r="341" spans="1:31" hidden="1">
       <c r="B341" t="s">
         <v>34</v>
       </c>
@@ -10402,7 +10058,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="342" spans="1:31">
+    <row r="342" spans="1:31" hidden="1">
       <c r="B342" t="s">
         <v>34</v>
       </c>
@@ -10425,7 +10081,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="343" spans="1:31">
+    <row r="343" spans="1:31" hidden="1">
       <c r="B343" t="s">
         <v>34</v>
       </c>
@@ -10451,7 +10107,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="344" spans="1:31">
+    <row r="344" spans="1:31" hidden="1">
       <c r="B344" t="s">
         <v>34</v>
       </c>
@@ -10480,7 +10136,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="345" spans="1:31">
+    <row r="345" spans="1:31" hidden="1">
       <c r="B345" t="s">
         <v>34</v>
       </c>
@@ -10521,7 +10177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:31">
+    <row r="346" spans="1:31" hidden="1">
       <c r="B346" t="s">
         <v>34</v>
       </c>
@@ -10544,7 +10200,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="347" spans="1:31">
+    <row r="347" spans="1:31" hidden="1">
       <c r="B347" t="s">
         <v>34</v>
       </c>
@@ -10582,7 +10238,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="348" spans="1:31">
+    <row r="348" spans="1:31" hidden="1">
       <c r="B348" t="s">
         <v>34</v>
       </c>
@@ -10606,7 +10262,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="349" spans="1:31">
+    <row r="349" spans="1:31" hidden="1">
       <c r="B349" t="s">
         <v>34</v>
       </c>
@@ -10638,7 +10294,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="350" spans="1:31">
+    <row r="350" spans="1:31" hidden="1">
       <c r="B350" t="s">
         <v>34</v>
       </c>
@@ -10676,7 +10332,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="351" spans="1:31">
+    <row r="351" spans="1:31" hidden="1">
       <c r="B351" t="s">
         <v>34</v>
       </c>
@@ -10708,7 +10364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:31">
+    <row r="352" spans="1:31" hidden="1">
       <c r="B352" t="s">
         <v>34</v>
       </c>
@@ -10731,7 +10387,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="353" spans="2:35">
+    <row r="353" spans="2:35" hidden="1">
       <c r="B353" t="s">
         <v>34</v>
       </c>
@@ -10766,7 +10422,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="354" spans="2:35">
+    <row r="354" spans="2:35" hidden="1">
       <c r="B354" t="s">
         <v>34</v>
       </c>
@@ -10795,7 +10451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="355" spans="2:35">
+    <row r="355" spans="2:35" hidden="1">
       <c r="B355" t="s">
         <v>34</v>
       </c>
@@ -10828,7 +10484,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="356" spans="2:35">
+    <row r="356" spans="2:35" hidden="1">
       <c r="B356" t="s">
         <v>34</v>
       </c>
@@ -10863,7 +10519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="2:35">
+    <row r="357" spans="2:35" hidden="1">
       <c r="B357" t="s">
         <v>34</v>
       </c>
@@ -10898,7 +10554,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="358" spans="2:35">
+    <row r="358" spans="2:35" hidden="1">
       <c r="B358" t="s">
         <v>34</v>
       </c>
@@ -10921,7 +10577,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="359" spans="2:35">
+    <row r="359" spans="2:35" hidden="1">
       <c r="B359" t="s">
         <v>34</v>
       </c>
@@ -10944,7 +10600,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="360" spans="2:35">
+    <row r="360" spans="2:35" hidden="1">
       <c r="B360" t="s">
         <v>34</v>
       </c>
@@ -10970,7 +10626,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="361" spans="2:35">
+    <row r="361" spans="2:35" hidden="1">
       <c r="B361" t="s">
         <v>34</v>
       </c>
@@ -10990,7 +10646,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="362" spans="2:35">
+    <row r="362" spans="2:35" hidden="1">
       <c r="B362" t="s">
         <v>34</v>
       </c>
@@ -11025,7 +10681,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="363" spans="2:35">
+    <row r="363" spans="2:35" hidden="1">
       <c r="B363" t="s">
         <v>34</v>
       </c>
@@ -11048,7 +10704,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="364" spans="2:35">
+    <row r="364" spans="2:35" hidden="1">
       <c r="B364" t="s">
         <v>34</v>
       </c>
@@ -11071,7 +10727,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="365" spans="2:35">
+    <row r="365" spans="2:35" hidden="1">
       <c r="B365" t="s">
         <v>34</v>
       </c>
@@ -11118,7 +10774,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="366" spans="2:35">
+    <row r="366" spans="2:35" hidden="1">
       <c r="B366" t="s">
         <v>34</v>
       </c>
@@ -11153,7 +10809,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="367" spans="2:35">
+    <row r="367" spans="2:35" hidden="1">
       <c r="B367" t="s">
         <v>34</v>
       </c>
@@ -11173,7 +10829,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="368" spans="2:35">
+    <row r="368" spans="2:35" hidden="1">
       <c r="B368" t="s">
         <v>34</v>
       </c>
@@ -11203,7 +10859,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="369" spans="2:34">
+    <row r="369" spans="2:34" hidden="1">
       <c r="B369" t="s">
         <v>34</v>
       </c>
@@ -11254,7 +10910,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="370" spans="2:34">
+    <row r="370" spans="2:34" hidden="1">
       <c r="B370" t="s">
         <v>34</v>
       </c>
@@ -11277,7 +10933,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="371" spans="2:34">
+    <row r="371" spans="2:34" hidden="1">
       <c r="B371" t="s">
         <v>34</v>
       </c>
@@ -11309,7 +10965,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="372" spans="2:34">
+    <row r="372" spans="2:34" hidden="1">
       <c r="B372" t="s">
         <v>34</v>
       </c>
@@ -11341,7 +10997,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="373" spans="2:34">
+    <row r="373" spans="2:34" hidden="1">
       <c r="B373" t="s">
         <v>34</v>
       </c>
@@ -11373,7 +11029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="374" spans="2:34">
+    <row r="374" spans="2:34" hidden="1">
       <c r="B374" t="s">
         <v>34</v>
       </c>
@@ -11442,9 +11098,6 @@
       <c r="AB375">
         <v>47</v>
       </c>
-      <c r="AC375">
-        <v>117</v>
-      </c>
     </row>
     <row r="376" spans="2:34">
       <c r="B376" t="s">
@@ -11471,9 +11124,6 @@
       <c r="AB376">
         <v>47</v>
       </c>
-      <c r="AC376">
-        <v>117</v>
-      </c>
     </row>
     <row r="377" spans="2:34">
       <c r="B377" t="s">
@@ -11509,9 +11159,6 @@
       <c r="AB377">
         <v>47</v>
       </c>
-      <c r="AC377">
-        <v>117</v>
-      </c>
     </row>
     <row r="378" spans="2:34">
       <c r="B378" t="s">
@@ -11544,9 +11191,6 @@
       <c r="AB378">
         <v>47</v>
       </c>
-      <c r="AC378">
-        <v>117</v>
-      </c>
     </row>
     <row r="379" spans="2:34">
       <c r="B379" t="s">
@@ -11567,9 +11211,6 @@
       <c r="AB379">
         <v>47</v>
       </c>
-      <c r="AC379">
-        <v>117</v>
-      </c>
     </row>
     <row r="380" spans="2:34">
       <c r="B380" t="s">
@@ -11590,9 +11231,6 @@
       <c r="AB380">
         <v>47</v>
       </c>
-      <c r="AC380">
-        <v>117</v>
-      </c>
     </row>
     <row r="381" spans="2:34">
       <c r="B381" t="s">
@@ -11613,9 +11251,6 @@
       <c r="AB381">
         <v>47</v>
       </c>
-      <c r="AC381">
-        <v>117</v>
-      </c>
     </row>
     <row r="382" spans="2:34">
       <c r="B382" t="s">
@@ -11639,9 +11274,6 @@
       <c r="AB382">
         <v>47</v>
       </c>
-      <c r="AC382">
-        <v>117</v>
-      </c>
     </row>
     <row r="383" spans="2:34">
       <c r="B383" t="s">
@@ -11677,9 +11309,6 @@
       <c r="AB383">
         <v>47</v>
       </c>
-      <c r="AC383">
-        <v>117</v>
-      </c>
       <c r="AD383">
         <v>5</v>
       </c>
@@ -11706,9 +11335,6 @@
       <c r="AB384">
         <v>47</v>
       </c>
-      <c r="AC384">
-        <v>117</v>
-      </c>
     </row>
     <row r="385" spans="2:35">
       <c r="B385" t="s">
@@ -11741,9 +11367,6 @@
       <c r="AB385">
         <v>47</v>
       </c>
-      <c r="AC385">
-        <v>117</v>
-      </c>
     </row>
     <row r="386" spans="2:35">
       <c r="B386" t="s">
@@ -11764,9 +11387,6 @@
       <c r="AB386">
         <v>47</v>
       </c>
-      <c r="AC386">
-        <v>117</v>
-      </c>
     </row>
     <row r="387" spans="2:35">
       <c r="B387" t="s">
@@ -11797,9 +11417,6 @@
       <c r="AB387">
         <v>47</v>
       </c>
-      <c r="AC387">
-        <v>117</v>
-      </c>
     </row>
     <row r="388" spans="2:35">
       <c r="B388" t="s">
@@ -11838,9 +11455,6 @@
       <c r="AB388">
         <v>47</v>
       </c>
-      <c r="AC388">
-        <v>117</v>
-      </c>
     </row>
     <row r="389" spans="2:35">
       <c r="B389" t="s">
@@ -11867,9 +11481,6 @@
       <c r="AB389">
         <v>47</v>
       </c>
-      <c r="AC389">
-        <v>117</v>
-      </c>
       <c r="AE389">
         <v>5</v>
       </c>
@@ -11908,9 +11519,6 @@
       <c r="AB390">
         <v>47</v>
       </c>
-      <c r="AC390">
-        <v>117</v>
-      </c>
     </row>
     <row r="391" spans="2:35">
       <c r="B391" t="s">
@@ -11937,9 +11545,6 @@
       <c r="AB391">
         <v>47</v>
       </c>
-      <c r="AC391">
-        <v>117</v>
-      </c>
     </row>
     <row r="392" spans="2:35">
       <c r="B392" t="s">
@@ -11963,9 +11568,6 @@
       <c r="AB392">
         <v>47</v>
       </c>
-      <c r="AC392">
-        <v>117</v>
-      </c>
       <c r="AI392">
         <v>5</v>
       </c>
@@ -11989,9 +11591,6 @@
       <c r="AB393">
         <v>47</v>
       </c>
-      <c r="AC393">
-        <v>117</v>
-      </c>
     </row>
     <row r="394" spans="2:35">
       <c r="B394" t="s">
@@ -12012,9 +11611,6 @@
       <c r="AB394">
         <v>47</v>
       </c>
-      <c r="AC394">
-        <v>117</v>
-      </c>
       <c r="AD394">
         <v>2</v>
       </c>
@@ -12050,9 +11646,6 @@
       <c r="AB395">
         <v>47</v>
       </c>
-      <c r="AC395">
-        <v>117</v>
-      </c>
     </row>
     <row r="396" spans="2:35">
       <c r="B396" t="s">
@@ -12079,9 +11672,6 @@
       <c r="AB396">
         <v>47</v>
       </c>
-      <c r="AC396">
-        <v>117</v>
-      </c>
     </row>
     <row r="397" spans="2:35">
       <c r="B397" t="s">
@@ -12102,9 +11692,6 @@
       <c r="AB397">
         <v>47</v>
       </c>
-      <c r="AC397">
-        <v>117</v>
-      </c>
     </row>
     <row r="398" spans="2:35">
       <c r="B398" t="s">
@@ -12125,9 +11712,6 @@
       <c r="AB398">
         <v>47</v>
       </c>
-      <c r="AC398">
-        <v>117</v>
-      </c>
     </row>
     <row r="399" spans="2:35">
       <c r="B399" t="s">
@@ -12160,9 +11744,6 @@
       <c r="AB399">
         <v>47</v>
       </c>
-      <c r="AC399">
-        <v>117</v>
-      </c>
     </row>
     <row r="400" spans="2:35">
       <c r="B400" t="s">
@@ -12183,9 +11764,6 @@
       <c r="AB400">
         <v>47</v>
       </c>
-      <c r="AC400">
-        <v>117</v>
-      </c>
     </row>
     <row r="401" spans="2:35">
       <c r="B401" t="s">
@@ -12230,9 +11808,6 @@
       <c r="AB401">
         <v>47</v>
       </c>
-      <c r="AC401">
-        <v>117</v>
-      </c>
     </row>
     <row r="402" spans="2:35">
       <c r="B402" t="s">
@@ -12253,9 +11828,6 @@
       <c r="AB402">
         <v>47</v>
       </c>
-      <c r="AC402">
-        <v>117</v>
-      </c>
       <c r="AD402">
         <v>1</v>
       </c>
@@ -12285,9 +11857,6 @@
       <c r="AB403">
         <v>47</v>
       </c>
-      <c r="AC403">
-        <v>117</v>
-      </c>
     </row>
     <row r="404" spans="2:35">
       <c r="B404" t="s">
@@ -12320,9 +11889,6 @@
       <c r="AB404">
         <v>47</v>
       </c>
-      <c r="AC404">
-        <v>117</v>
-      </c>
     </row>
     <row r="405" spans="2:35">
       <c r="B405" t="s">
@@ -12343,9 +11909,6 @@
       <c r="AB405">
         <v>47</v>
       </c>
-      <c r="AC405">
-        <v>117</v>
-      </c>
     </row>
     <row r="406" spans="2:35">
       <c r="B406" t="s">
@@ -12378,9 +11941,6 @@
       <c r="AB406">
         <v>47</v>
       </c>
-      <c r="AC406">
-        <v>117</v>
-      </c>
     </row>
     <row r="407" spans="2:35">
       <c r="B407" t="s">
@@ -12401,9 +11961,6 @@
       <c r="AB407">
         <v>47</v>
       </c>
-      <c r="AC407">
-        <v>117</v>
-      </c>
     </row>
     <row r="408" spans="2:35">
       <c r="B408" t="s">
@@ -12424,9 +11981,6 @@
       <c r="AB408">
         <v>47</v>
       </c>
-      <c r="AC408">
-        <v>117</v>
-      </c>
     </row>
     <row r="409" spans="2:35">
       <c r="B409" t="s">
@@ -12451,9 +12005,6 @@
       <c r="AB409">
         <v>47</v>
       </c>
-      <c r="AC409">
-        <v>117</v>
-      </c>
     </row>
     <row r="410" spans="2:35">
       <c r="B410" t="s">
@@ -12477,9 +12028,6 @@
       <c r="AB410">
         <v>47</v>
       </c>
-      <c r="AC410">
-        <v>117</v>
-      </c>
     </row>
     <row r="411" spans="2:35">
       <c r="B411" t="s">
@@ -12515,9 +12063,6 @@
       <c r="AB411">
         <v>47</v>
       </c>
-      <c r="AC411">
-        <v>117</v>
-      </c>
       <c r="AF411">
         <v>14</v>
       </c>
@@ -12572,9 +12117,6 @@
       <c r="AB412">
         <v>47</v>
       </c>
-      <c r="AC412">
-        <v>117</v>
-      </c>
       <c r="AG412">
         <v>7.3</v>
       </c>
@@ -12582,7 +12124,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="413" spans="2:35">
+    <row r="413" spans="2:35" hidden="1">
       <c r="B413" t="s">
         <v>17</v>
       </c>
@@ -12605,7 +12147,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="414" spans="2:35">
+    <row r="414" spans="2:35" hidden="1">
       <c r="B414" t="s">
         <v>17</v>
       </c>
@@ -12628,7 +12170,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="415" spans="2:35">
+    <row r="415" spans="2:35" hidden="1">
       <c r="B415" t="s">
         <v>17</v>
       </c>
@@ -12654,7 +12196,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="416" spans="2:35">
+    <row r="416" spans="2:35" hidden="1">
       <c r="B416" t="s">
         <v>17</v>
       </c>
@@ -12677,7 +12219,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="417" spans="2:35">
+    <row r="417" spans="2:35" hidden="1">
       <c r="B417" t="s">
         <v>17</v>
       </c>
@@ -12700,7 +12242,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="418" spans="2:35">
+    <row r="418" spans="2:35" hidden="1">
       <c r="B418" t="s">
         <v>17</v>
       </c>
@@ -12726,7 +12268,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="419" spans="2:35">
+    <row r="419" spans="2:35" hidden="1">
       <c r="B419" t="s">
         <v>17</v>
       </c>
@@ -12752,7 +12294,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="420" spans="2:35">
+    <row r="420" spans="2:35" hidden="1">
       <c r="B420" t="s">
         <v>17</v>
       </c>
@@ -12775,7 +12317,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="421" spans="2:35">
+    <row r="421" spans="2:35" hidden="1">
       <c r="B421" t="s">
         <v>17</v>
       </c>
@@ -12798,7 +12340,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="422" spans="2:35">
+    <row r="422" spans="2:35" hidden="1">
       <c r="B422" t="s">
         <v>14</v>
       </c>
@@ -12821,7 +12363,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="423" spans="2:35">
+    <row r="423" spans="2:35" hidden="1">
       <c r="B423" t="s">
         <v>14</v>
       </c>
@@ -12844,7 +12386,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="424" spans="2:35">
+    <row r="424" spans="2:35" hidden="1">
       <c r="B424" t="s">
         <v>14</v>
       </c>
@@ -12870,7 +12412,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="425" spans="2:35">
+    <row r="425" spans="2:35" hidden="1">
       <c r="B425" t="s">
         <v>14</v>
       </c>
@@ -12893,7 +12435,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="426" spans="2:35">
+    <row r="426" spans="2:35" hidden="1">
       <c r="B426" t="s">
         <v>14</v>
       </c>
@@ -12916,7 +12458,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="427" spans="2:35">
+    <row r="427" spans="2:35" hidden="1">
       <c r="B427" t="s">
         <v>14</v>
       </c>
@@ -12939,7 +12481,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="428" spans="2:35">
+    <row r="428" spans="2:35" hidden="1">
       <c r="B428" t="s">
         <v>14</v>
       </c>
@@ -12965,7 +12507,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="429" spans="2:35">
+    <row r="429" spans="2:35" hidden="1">
       <c r="B429" t="s">
         <v>14</v>
       </c>
@@ -12994,7 +12536,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="430" spans="2:35">
+    <row r="430" spans="2:35" hidden="1">
       <c r="B430" t="s">
         <v>14</v>
       </c>
@@ -13023,7 +12565,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="431" spans="2:35">
+    <row r="431" spans="2:35" hidden="1">
       <c r="B431" t="s">
         <v>14</v>
       </c>
@@ -13046,7 +12588,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="432" spans="2:35">
+    <row r="432" spans="2:35" hidden="1">
       <c r="B432" t="s">
         <v>14</v>
       </c>
@@ -13069,7 +12611,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="433" spans="2:35">
+    <row r="433" spans="2:35" hidden="1">
       <c r="B433" t="s">
         <v>14</v>
       </c>
@@ -13092,7 +12634,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="434" spans="2:35">
+    <row r="434" spans="2:35" hidden="1">
       <c r="B434" t="s">
         <v>14</v>
       </c>
@@ -13115,7 +12657,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="435" spans="2:35">
+    <row r="435" spans="2:35" hidden="1">
       <c r="B435" t="s">
         <v>14</v>
       </c>
@@ -13139,7 +12681,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="436" spans="2:35">
+    <row r="436" spans="2:35" hidden="1">
       <c r="B436" t="s">
         <v>14</v>
       </c>
@@ -13165,7 +12707,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="437" spans="2:35">
+    <row r="437" spans="2:35" hidden="1">
       <c r="B437" t="s">
         <v>14</v>
       </c>
@@ -13188,7 +12730,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="438" spans="2:35">
+    <row r="438" spans="2:35" hidden="1">
       <c r="B438" t="s">
         <v>14</v>
       </c>
@@ -13214,7 +12756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="439" spans="2:35">
+    <row r="439" spans="2:35" hidden="1">
       <c r="B439" t="s">
         <v>14</v>
       </c>
@@ -13238,7 +12780,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="440" spans="2:35">
+    <row r="440" spans="2:35" hidden="1">
       <c r="B440" t="s">
         <v>14</v>
       </c>
@@ -13261,7 +12803,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="441" spans="2:35">
+    <row r="441" spans="2:35" hidden="1">
       <c r="B441" t="s">
         <v>14</v>
       </c>
@@ -13284,7 +12826,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="442" spans="2:35">
+    <row r="442" spans="2:35" hidden="1">
       <c r="B442" t="s">
         <v>14</v>
       </c>
@@ -13310,7 +12852,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="443" spans="2:35">
+    <row r="443" spans="2:35" hidden="1">
       <c r="B443" t="s">
         <v>18</v>
       </c>
@@ -13336,7 +12878,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="444" spans="2:35">
+    <row r="444" spans="2:35" hidden="1">
       <c r="B444" t="s">
         <v>18</v>
       </c>
@@ -13359,7 +12901,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="445" spans="2:35">
+    <row r="445" spans="2:35" hidden="1">
       <c r="B445" t="s">
         <v>18</v>
       </c>
@@ -13382,7 +12924,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="446" spans="2:35">
+    <row r="446" spans="2:35" hidden="1">
       <c r="B446" t="s">
         <v>18</v>
       </c>
@@ -13411,7 +12953,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="447" spans="2:35">
+    <row r="447" spans="2:35" hidden="1">
       <c r="B447" t="s">
         <v>18</v>
       </c>
@@ -13435,7 +12977,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="448" spans="2:35">
+    <row r="448" spans="2:35" hidden="1">
       <c r="B448" t="s">
         <v>18</v>
       </c>
@@ -13467,7 +13009,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="449" spans="2:35">
+    <row r="449" spans="2:35" hidden="1">
       <c r="B449" t="s">
         <v>18</v>
       </c>
@@ -13494,7 +13036,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="450" spans="2:35">
+    <row r="450" spans="2:35" hidden="1">
       <c r="B450" t="s">
         <v>18</v>
       </c>
@@ -13520,7 +13062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="451" spans="2:35">
+    <row r="451" spans="2:35" hidden="1">
       <c r="B451" t="s">
         <v>18</v>
       </c>
@@ -13540,7 +13082,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="452" spans="2:35">
+    <row r="452" spans="2:35" hidden="1">
       <c r="B452" t="s">
         <v>18</v>
       </c>
@@ -13564,7 +13106,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="453" spans="2:35">
+    <row r="453" spans="2:35" hidden="1">
       <c r="B453" t="s">
         <v>18</v>
       </c>
@@ -13587,7 +13129,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="454" spans="2:35">
+    <row r="454" spans="2:35" hidden="1">
       <c r="B454" t="s">
         <v>18</v>
       </c>
@@ -13614,7 +13156,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="455" spans="2:35">
+    <row r="455" spans="2:35" hidden="1">
       <c r="B455" t="s">
         <v>18</v>
       </c>
@@ -13637,7 +13179,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="456" spans="2:35">
+    <row r="456" spans="2:35" hidden="1">
       <c r="B456" t="s">
         <v>18</v>
       </c>
@@ -13660,7 +13202,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="457" spans="2:35">
+    <row r="457" spans="2:35" hidden="1">
       <c r="B457" t="s">
         <v>23</v>
       </c>
@@ -13683,7 +13225,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="458" spans="2:35">
+    <row r="458" spans="2:35" hidden="1">
       <c r="B458" t="s">
         <v>23</v>
       </c>
@@ -13706,7 +13248,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="459" spans="2:35">
+    <row r="459" spans="2:35" hidden="1">
       <c r="B459" t="s">
         <v>23</v>
       </c>
@@ -13735,7 +13277,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="460" spans="2:35">
+    <row r="460" spans="2:35" hidden="1">
       <c r="B460" t="s">
         <v>23</v>
       </c>
@@ -13804,7 +13346,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="461" spans="2:35">
+    <row r="461" spans="2:35" hidden="1">
       <c r="B461" t="s">
         <v>24</v>
       </c>
@@ -13830,7 +13372,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="462" spans="2:35">
+    <row r="462" spans="2:35" hidden="1">
       <c r="B462" t="s">
         <v>24</v>
       </c>
@@ -13853,7 +13395,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="463" spans="2:35">
+    <row r="463" spans="2:35" hidden="1">
       <c r="B463" t="s">
         <v>24</v>
       </c>
@@ -13888,7 +13430,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="464" spans="2:35">
+    <row r="464" spans="2:35" hidden="1">
       <c r="B464" t="s">
         <v>24</v>
       </c>
@@ -13923,7 +13465,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="465" spans="2:35">
+    <row r="465" spans="2:35" hidden="1">
       <c r="B465" t="s">
         <v>24</v>
       </c>
@@ -13946,7 +13488,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="466" spans="2:35">
+    <row r="466" spans="2:35" hidden="1">
       <c r="B466" t="s">
         <v>24</v>
       </c>
@@ -13981,7 +13523,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="467" spans="2:35">
+    <row r="467" spans="2:35" hidden="1">
       <c r="B467" t="s">
         <v>24</v>
       </c>
@@ -14004,7 +13546,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="468" spans="2:35">
+    <row r="468" spans="2:35" hidden="1">
       <c r="B468" t="s">
         <v>24</v>
       </c>
@@ -14042,7 +13584,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="469" spans="2:35">
+    <row r="469" spans="2:35" hidden="1">
       <c r="B469" t="s">
         <v>24</v>
       </c>
@@ -14099,7 +13641,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="470" spans="2:35">
+    <row r="470" spans="2:35" hidden="1">
       <c r="B470" t="s">
         <v>24</v>
       </c>
@@ -14128,7 +13670,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="471" spans="2:35">
+    <row r="471" spans="2:35" hidden="1">
       <c r="B471" t="s">
         <v>25</v>
       </c>
@@ -14151,7 +13693,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="472" spans="2:35">
+    <row r="472" spans="2:35" hidden="1">
       <c r="B472" t="s">
         <v>25</v>
       </c>
@@ -14191,7 +13733,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="473" spans="2:35">
+    <row r="473" spans="2:35" hidden="1">
       <c r="B473" t="s">
         <v>25</v>
       </c>
@@ -14224,7 +13766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="474" spans="2:35">
+    <row r="474" spans="2:35" hidden="1">
       <c r="B474" t="s">
         <v>25</v>
       </c>
@@ -14250,7 +13792,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="475" spans="2:35">
+    <row r="475" spans="2:35" hidden="1">
       <c r="B475" t="s">
         <v>25</v>
       </c>
@@ -14273,7 +13815,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="476" spans="2:35">
+    <row r="476" spans="2:35" hidden="1">
       <c r="B476" t="s">
         <v>25</v>
       </c>
@@ -14302,7 +13844,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="477" spans="2:35">
+    <row r="477" spans="2:35" hidden="1">
       <c r="B477" t="s">
         <v>25</v>
       </c>
@@ -14328,7 +13870,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="478" spans="2:35">
+    <row r="478" spans="2:35" hidden="1">
       <c r="B478" t="s">
         <v>25</v>
       </c>
@@ -14388,7 +13930,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="479" spans="2:35">
+    <row r="479" spans="2:35" hidden="1">
       <c r="B479" t="s">
         <v>25</v>
       </c>
@@ -14430,9 +13972,6 @@
       <c r="AB480">
         <v>49</v>
       </c>
-      <c r="AC480">
-        <v>111</v>
-      </c>
     </row>
     <row r="481" spans="2:35">
       <c r="B481" t="s">
@@ -14453,9 +13992,6 @@
       <c r="AB481">
         <v>49</v>
       </c>
-      <c r="AC481">
-        <v>111</v>
-      </c>
     </row>
     <row r="482" spans="2:35">
       <c r="B482" t="s">
@@ -14476,9 +14012,6 @@
       <c r="AB482">
         <v>49</v>
       </c>
-      <c r="AC482">
-        <v>111</v>
-      </c>
     </row>
     <row r="483" spans="2:35">
       <c r="B483" t="s">
@@ -14496,9 +14029,6 @@
       <c r="AB483">
         <v>49</v>
       </c>
-      <c r="AC483">
-        <v>111</v>
-      </c>
     </row>
     <row r="484" spans="2:35">
       <c r="B484" t="s">
@@ -14525,9 +14055,6 @@
       <c r="AB484">
         <v>49</v>
       </c>
-      <c r="AC484">
-        <v>111</v>
-      </c>
     </row>
     <row r="485" spans="2:35">
       <c r="B485" t="s">
@@ -14588,9 +14115,6 @@
       <c r="AB485">
         <v>49</v>
       </c>
-      <c r="AC485">
-        <v>111</v>
-      </c>
       <c r="AG485">
         <v>7.2</v>
       </c>
@@ -14623,9 +14147,6 @@
       <c r="AB486">
         <v>49</v>
       </c>
-      <c r="AC486">
-        <v>98</v>
-      </c>
       <c r="AI486">
         <v>5</v>
       </c>
@@ -14661,9 +14182,6 @@
       <c r="AB487">
         <v>49</v>
       </c>
-      <c r="AC487">
-        <v>98</v>
-      </c>
     </row>
     <row r="488" spans="2:35">
       <c r="B488" t="s">
@@ -14684,9 +14202,6 @@
       <c r="AB488">
         <v>49</v>
       </c>
-      <c r="AC488">
-        <v>98</v>
-      </c>
     </row>
     <row r="489" spans="2:35">
       <c r="B489" t="s">
@@ -14719,9 +14234,6 @@
       <c r="AB489">
         <v>49</v>
       </c>
-      <c r="AC489">
-        <v>98</v>
-      </c>
     </row>
     <row r="490" spans="2:35">
       <c r="B490" t="s">
@@ -14742,9 +14254,6 @@
       <c r="AB490">
         <v>49</v>
       </c>
-      <c r="AC490">
-        <v>98</v>
-      </c>
     </row>
     <row r="491" spans="2:35">
       <c r="B491" t="s">
@@ -14777,9 +14286,6 @@
       <c r="AB491">
         <v>49</v>
       </c>
-      <c r="AC491">
-        <v>98</v>
-      </c>
     </row>
     <row r="492" spans="2:35">
       <c r="B492" t="s">
@@ -14800,9 +14306,6 @@
       <c r="AB492">
         <v>49</v>
       </c>
-      <c r="AC492">
-        <v>98</v>
-      </c>
     </row>
     <row r="493" spans="2:35">
       <c r="B493" t="s">
@@ -14823,9 +14326,6 @@
       <c r="AB493">
         <v>49</v>
       </c>
-      <c r="AC493">
-        <v>98</v>
-      </c>
     </row>
     <row r="494" spans="2:35">
       <c r="B494" t="s">
@@ -14855,9 +14355,6 @@
       <c r="AB494">
         <v>49</v>
       </c>
-      <c r="AC494">
-        <v>98</v>
-      </c>
     </row>
     <row r="495" spans="2:35">
       <c r="B495" t="s">
@@ -14912,9 +14409,6 @@
       <c r="AB495">
         <v>49</v>
       </c>
-      <c r="AC495">
-        <v>98</v>
-      </c>
       <c r="AG495">
         <v>6.8</v>
       </c>
@@ -14941,9 +14435,6 @@
       <c r="AB496">
         <v>49</v>
       </c>
-      <c r="AC496">
-        <v>91</v>
-      </c>
     </row>
     <row r="497" spans="2:35">
       <c r="B497" t="s">
@@ -14969,9 +14460,6 @@
       </c>
       <c r="AB497">
         <v>49</v>
-      </c>
-      <c r="AC497">
-        <v>91</v>
       </c>
     </row>
     <row r="498" spans="2:35">
@@ -14995,9 +14483,6 @@
       <c r="AB498">
         <v>49</v>
       </c>
-      <c r="AC498">
-        <v>91</v>
-      </c>
     </row>
     <row r="499" spans="2:35">
       <c r="B499" t="s">
@@ -15018,9 +14503,6 @@
       <c r="AB499">
         <v>49</v>
       </c>
-      <c r="AC499">
-        <v>91</v>
-      </c>
     </row>
     <row r="500" spans="2:35">
       <c r="B500" t="s">
@@ -15050,9 +14532,6 @@
       <c r="AB500">
         <v>49</v>
       </c>
-      <c r="AC500">
-        <v>91</v>
-      </c>
     </row>
     <row r="501" spans="2:35">
       <c r="B501" t="s">
@@ -15088,9 +14567,6 @@
       <c r="AB501">
         <v>49</v>
       </c>
-      <c r="AC501">
-        <v>91</v>
-      </c>
     </row>
     <row r="502" spans="2:35">
       <c r="B502" t="s">
@@ -15114,9 +14590,6 @@
       <c r="AB502">
         <v>49</v>
       </c>
-      <c r="AC502">
-        <v>91</v>
-      </c>
       <c r="AI502">
         <v>0.8</v>
       </c>
@@ -15140,9 +14613,6 @@
       <c r="AB503">
         <v>49</v>
       </c>
-      <c r="AC503">
-        <v>91</v>
-      </c>
     </row>
     <row r="504" spans="2:35">
       <c r="B504" t="s">
@@ -15163,9 +14633,6 @@
       <c r="AB504">
         <v>49</v>
       </c>
-      <c r="AC504">
-        <v>91</v>
-      </c>
     </row>
     <row r="505" spans="2:35">
       <c r="B505" t="s">
@@ -15186,9 +14653,6 @@
       <c r="AB505">
         <v>49</v>
       </c>
-      <c r="AC505">
-        <v>91</v>
-      </c>
     </row>
     <row r="506" spans="2:35">
       <c r="B506" t="s">
@@ -15209,11 +14673,8 @@
       <c r="AB506">
         <v>49</v>
       </c>
-      <c r="AC506">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="507" spans="2:35">
+    </row>
+    <row r="507" spans="2:35" hidden="1">
       <c r="B507" t="s">
         <v>15</v>
       </c>
@@ -15236,7 +14697,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="508" spans="2:35">
+    <row r="508" spans="2:35" hidden="1">
       <c r="B508" t="s">
         <v>15</v>
       </c>
@@ -15251,7 +14712,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="509" spans="2:35">
+    <row r="509" spans="2:35" hidden="1">
       <c r="B509" t="s">
         <v>15</v>
       </c>
@@ -15277,7 +14738,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="510" spans="2:35">
+    <row r="510" spans="2:35" hidden="1">
       <c r="B510" t="s">
         <v>15</v>
       </c>
@@ -15303,7 +14764,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="511" spans="2:35">
+    <row r="511" spans="2:35" hidden="1">
       <c r="B511" t="s">
         <v>15</v>
       </c>
@@ -15330,7 +14791,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="512" spans="2:35">
+    <row r="512" spans="2:35" hidden="1">
       <c r="B512" t="s">
         <v>15</v>
       </c>
@@ -15353,7 +14814,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="513" spans="2:35">
+    <row r="513" spans="2:35" hidden="1">
       <c r="B513" t="s">
         <v>15</v>
       </c>
@@ -15376,7 +14837,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="514" spans="2:35">
+    <row r="514" spans="2:35" hidden="1">
       <c r="B514" t="s">
         <v>16</v>
       </c>
@@ -15430,7 +14891,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="515" spans="2:35">
+    <row r="515" spans="2:35" hidden="1">
       <c r="B515" t="s">
         <v>16</v>
       </c>
@@ -15456,7 +14917,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="516" spans="2:35">
+    <row r="516" spans="2:35" hidden="1">
       <c r="B516" t="s">
         <v>16</v>
       </c>
@@ -15482,7 +14943,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="517" spans="2:35">
+    <row r="517" spans="2:35" hidden="1">
       <c r="B517" t="s">
         <v>16</v>
       </c>
@@ -15515,7 +14976,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="518" spans="2:35">
+    <row r="518" spans="2:35" hidden="1">
       <c r="B518" t="s">
         <v>16</v>
       </c>
@@ -15538,7 +14999,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="519" spans="2:35">
+    <row r="519" spans="2:35" hidden="1">
       <c r="B519" t="s">
         <v>16</v>
       </c>
@@ -15564,7 +15025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="520" spans="2:35">
+    <row r="520" spans="2:35" hidden="1">
       <c r="B520" t="s">
         <v>16</v>
       </c>
@@ -15587,7 +15048,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="521" spans="2:35">
+    <row r="521" spans="2:35" hidden="1">
       <c r="B521" t="s">
         <v>16</v>
       </c>
@@ -15613,7 +15074,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="522" spans="2:35">
+    <row r="522" spans="2:35" hidden="1">
       <c r="B522" t="s">
         <v>16</v>
       </c>
@@ -15636,7 +15097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="523" spans="2:35">
+    <row r="523" spans="2:35" hidden="1">
       <c r="B523" t="s">
         <v>16</v>
       </c>
@@ -15659,7 +15120,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="524" spans="2:35">
+    <row r="524" spans="2:35" hidden="1">
       <c r="B524" t="s">
         <v>16</v>
       </c>
@@ -15688,7 +15149,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="525" spans="2:35">
+    <row r="525" spans="2:35" hidden="1">
       <c r="B525" t="s">
         <v>16</v>
       </c>
@@ -15724,7 +15185,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="526" spans="2:35">
+    <row r="526" spans="2:35" hidden="1">
       <c r="B526" t="s">
         <v>16</v>
       </c>
@@ -15751,7 +15212,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="527" spans="2:35">
+    <row r="527" spans="2:35" hidden="1">
       <c r="B527" t="s">
         <v>19</v>
       </c>
@@ -15775,7 +15236,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="528" spans="2:35">
+    <row r="528" spans="2:35" hidden="1">
       <c r="B528" t="s">
         <v>19</v>
       </c>
@@ -15799,7 +15260,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="529" spans="2:34">
+    <row r="529" spans="2:34" hidden="1">
       <c r="B529" t="s">
         <v>19</v>
       </c>
@@ -15826,7 +15287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="530" spans="2:34">
+    <row r="530" spans="2:34" hidden="1">
       <c r="B530" t="s">
         <v>19</v>
       </c>
@@ -15854,7 +15315,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="531" spans="2:34">
+    <row r="531" spans="2:34" hidden="1">
       <c r="B531" t="s">
         <v>19</v>
       </c>
@@ -15877,7 +15338,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="532" spans="2:34">
+    <row r="532" spans="2:34" hidden="1">
       <c r="B532" t="s">
         <v>19</v>
       </c>
@@ -15900,7 +15361,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="533" spans="2:34">
+    <row r="533" spans="2:34" hidden="1">
       <c r="B533" t="s">
         <v>19</v>
       </c>
@@ -15926,7 +15387,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="534" spans="2:34">
+    <row r="534" spans="2:34" hidden="1">
       <c r="B534" t="s">
         <v>19</v>
       </c>
@@ -15949,7 +15410,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="535" spans="2:34">
+    <row r="535" spans="2:34" hidden="1">
       <c r="B535" t="s">
         <v>19</v>
       </c>
@@ -15978,7 +15439,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="536" spans="2:34">
+    <row r="536" spans="2:34" hidden="1">
       <c r="B536" t="s">
         <v>19</v>
       </c>
@@ -16119,6 +15580,18 @@
       <c r="T574" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI536" xr:uid="{21C69D9A-1FFA-4799-BC03-A6694D3363DD}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="exp1EmeraldWaterIrr"/>
+        <filter val="exp1EmeraldWaterPodIrr"/>
+        <filter val="exp1EmeraldWaterRF"/>
+        <filter val="exp2WaterIrrCultivarEmerald"/>
+        <filter val="exp2WaterRFCultivarEmerald"/>
+        <filter val="exp2WaterTermStressCultivarEmerald"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI541">
     <sortCondition descending="1" ref="R2:R541"/>
   </sortState>

</xml_diff>